<commit_message>
Turbo Mode Added, DTC JASSM Summary match added
</commit_message>
<xml_diff>
--- a/Debrief Sheet Template v4.xlsx
+++ b/Debrief Sheet Template v4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Python\bidds-debrief\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC486648-F768-421C-9F60-1079510D723C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AFCBED-A113-4338-A85A-9F967373EF36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4470" yWindow="2115" windowWidth="24660" windowHeight="17235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Debrief" sheetId="1" r:id="rId1"/>
@@ -484,15 +484,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="d\ mmm\ yy"/>
     <numFmt numFmtId="165" formatCode="hhmm:ss"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="167" formatCode="0\I"/>
-    <numFmt numFmtId="170" formatCode="0\ \'"/>
-    <numFmt numFmtId="171" formatCode="000&quot; TK&quot;"/>
-    <numFmt numFmtId="172" formatCode="000&quot; MH&quot;"/>
-    <numFmt numFmtId="173" formatCode="dd\ mmm\ yy"/>
+    <numFmt numFmtId="168" formatCode="0\ \'"/>
+    <numFmt numFmtId="169" formatCode="000&quot; TK&quot;"/>
+    <numFmt numFmtId="170" formatCode="000&quot; MH&quot;"/>
+    <numFmt numFmtId="171" formatCode="dd\ mmm\ yy"/>
+    <numFmt numFmtId="172" formatCode="0000"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -1346,7 +1347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1438,10 +1439,10 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="9" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="9" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="9" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="9" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1484,20 +1485,20 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="9" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="9" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="9" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="9" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="9" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="9" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="9" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="9" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1525,105 +1526,119 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="9" fillId="8" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="172" fontId="9" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
@@ -1635,110 +1650,210 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="8" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="26" formatCode="h:mm:ss"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1815,60 +1930,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1888,17 +1949,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="S5:T17" headerRowCount="0" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="S5:T17" headerRowCount="0" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" headerRowDxfId="4" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" headerRowDxfId="2" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" headerRowDxfId="17" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" headerRowDxfId="15" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:AC100" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:AC100" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A1:AC100" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="29">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Record Number"/>
@@ -1908,7 +1969,7 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="TOT"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="TOR"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="BULL"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="TOF"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="TOF" dataDxfId="12"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="WPN Type"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="TGT Name"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="TGT LAT"/>
@@ -2262,7 +2323,7 @@
   <dimension ref="A1:AB89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P38" sqref="P38"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2283,107 +2344,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="141" t="str">
+      <c r="A1" s="109" t="str">
         <f>IF(ISBLANK(cs),"",cs)</f>
         <v/>
       </c>
-      <c r="B1" s="142"/>
-      <c r="C1" s="143" t="s">
+      <c r="B1" s="110"/>
+      <c r="C1" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
       <c r="F1" s="64"/>
       <c r="G1" s="65"/>
       <c r="H1" s="63"/>
-      <c r="I1" s="71" t="s">
+      <c r="I1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="116"/>
-      <c r="K1" s="116"/>
-      <c r="L1" s="116"/>
-      <c r="M1" s="116"/>
-      <c r="N1" s="116"/>
-      <c r="O1" s="117"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="80"/>
     </row>
     <row r="2" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="128" t="str">
+      <c r="A2" s="95" t="str">
         <f>IF(msndate=0,"",msndate)</f>
         <v/>
       </c>
-      <c r="B2" s="129"/>
-      <c r="C2" s="133" t="s">
+      <c r="B2" s="96"/>
+      <c r="C2" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="134"/>
+      <c r="D2" s="102"/>
       <c r="E2" s="9" t="str">
         <f>IF(ISBLANK(msnlead),"",msnlead)</f>
         <v/>
       </c>
-      <c r="F2" s="125" t="s">
+      <c r="F2" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="106"/>
+      <c r="G2" s="92"/>
       <c r="H2" s="63"/>
-      <c r="I2" s="118" t="s">
+      <c r="I2" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="119"/>
-      <c r="K2" s="137" t="str">
+      <c r="J2" s="82"/>
+      <c r="K2" s="105" t="str">
         <f>IF(ISBLANK(tgp),"",tgp)</f>
         <v>SNIPER</v>
       </c>
-      <c r="L2" s="119"/>
+      <c r="L2" s="82"/>
       <c r="M2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="120" t="str">
+      <c r="N2" s="83" t="str">
         <f>IF(ISBLANK(dtcsortie),"",dtcsortie)</f>
         <v/>
       </c>
-      <c r="O2" s="102"/>
+      <c r="O2" s="84"/>
     </row>
     <row r="3" spans="1:28" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="130" t="str">
+      <c r="A3" s="97" t="str">
         <f>IF(msnnum=0,"",msnnum)</f>
         <v/>
       </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="135" t="s">
+      <c r="B3" s="98"/>
+      <c r="C3" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="136"/>
+      <c r="D3" s="104"/>
       <c r="E3" s="66" t="str">
         <f>IF(ISBLANK(msnwso),"",msnwso)</f>
         <v/>
       </c>
-      <c r="F3" s="124" t="str">
+      <c r="F3" s="89" t="str">
         <f>IF(ISBLANK(Combined!B2),"",Combined!B2)</f>
         <v/>
       </c>
-      <c r="G3" s="123"/>
+      <c r="G3" s="90"/>
       <c r="H3" s="63"/>
-      <c r="I3" s="121" t="s">
+      <c r="I3" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="90"/>
-      <c r="K3" s="138" t="str">
+      <c r="J3" s="86"/>
+      <c r="K3" s="106" t="str">
         <f>IF(ISBLANK(tgpserial),"",tgpserial)</f>
         <v/>
       </c>
-      <c r="L3" s="90"/>
+      <c r="L3" s="86"/>
       <c r="M3" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="122" t="str">
+      <c r="N3" s="87" t="str">
         <f>IF(ISBLANK(dtcmission),"",dtcmission)</f>
         <v/>
       </c>
-      <c r="O3" s="123"/>
-      <c r="S3" s="86" t="s">
+      <c r="O3" s="88"/>
+      <c r="S3" s="152" t="s">
         <v>130</v>
       </c>
-      <c r="T3" s="86"/>
+      <c r="T3" s="152"/>
       <c r="V3" s="1" t="s">
         <v>10</v>
       </c>
@@ -2410,10 +2471,10 @@
       <c r="E4" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="139" t="s">
+      <c r="F4" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="140"/>
+      <c r="G4" s="108"/>
       <c r="I4" s="46" t="s">
         <v>18</v>
       </c>
@@ -2442,8 +2503,8 @@
         <v>25</v>
       </c>
       <c r="R4" s="5"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
+      <c r="S4" s="152"/>
+      <c r="T4" s="152"/>
       <c r="V4" t="s">
         <v>27</v>
       </c>
@@ -2464,14 +2525,14 @@
       <c r="B5" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="131" t="s">
+      <c r="C5" s="99" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="132"/>
-      <c r="E5" s="126" t="s">
+      <c r="D5" s="100"/>
+      <c r="E5" s="93" t="s">
         <v>132</v>
       </c>
-      <c r="F5" s="127"/>
+      <c r="F5" s="94"/>
       <c r="G5" s="45" t="s">
         <v>33</v>
       </c>
@@ -2484,11 +2545,11 @@
       <c r="K5" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="L5" s="144" t="s">
+      <c r="L5" s="112" t="s">
         <v>134</v>
       </c>
-      <c r="M5" s="145"/>
-      <c r="N5" s="146"/>
+      <c r="M5" s="113"/>
+      <c r="N5" s="114"/>
       <c r="O5" s="45" t="s">
         <v>40</v>
       </c>
@@ -2537,11 +2598,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A7)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A7)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F6" s="103" t="str">
+      <c r="F6" s="127" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A7)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A7)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G6" s="102"/>
+      <c r="G6" s="84"/>
       <c r="H6" s="39"/>
       <c r="I6" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A7)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A7)-ROW($A$7)+2)/2,0))</f>
@@ -2597,16 +2658,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A7)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A7)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C7" s="87" t="str">
+      <c r="C7" s="130" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A7)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A7)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D7" s="88"/>
-      <c r="E7" s="89" t="str">
+      <c r="D7" s="98"/>
+      <c r="E7" s="131" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A7)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A7)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A7)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F7" s="90"/>
+      <c r="F7" s="86"/>
       <c r="G7" s="35" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A7)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A7)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -2624,12 +2685,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A7)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A7)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L7" s="147" t="str">
+      <c r="L7" s="72" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A7)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A7)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A7)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A7)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A7)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M7" s="148"/>
-      <c r="N7" s="149"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="74"/>
       <c r="O7" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A7)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A7)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -2669,11 +2730,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A9)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A9)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F8" s="101" t="str">
+      <c r="F8" s="126" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A9)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A9)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G8" s="102"/>
+      <c r="G8" s="84"/>
       <c r="H8" s="39"/>
       <c r="I8" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A9)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A9)-ROW($A$7)+2)/2,0))</f>
@@ -2729,16 +2790,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A9)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A9)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C9" s="91" t="str">
+      <c r="C9" s="128" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A9)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A9)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D9" s="88"/>
-      <c r="E9" s="92" t="str">
+      <c r="D9" s="98"/>
+      <c r="E9" s="129" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A9)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A9)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A9)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F9" s="90"/>
+      <c r="F9" s="86"/>
       <c r="G9" s="36" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A9)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A9)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -2756,12 +2817,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A9)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A9)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L9" s="150" t="str">
+      <c r="L9" s="75" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A9)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A9)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A9)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A9)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A9)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M9" s="151"/>
-      <c r="N9" s="152"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="77"/>
       <c r="O9" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A9)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A9)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -2798,11 +2859,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A11)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A11)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F10" s="103" t="str">
+      <c r="F10" s="127" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A11)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A11)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G10" s="102"/>
+      <c r="G10" s="84"/>
       <c r="H10" s="39"/>
       <c r="I10" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A11)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A11)-ROW($A$7)+2)/2,0))</f>
@@ -2857,16 +2918,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A11)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A11)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C11" s="87" t="str">
+      <c r="C11" s="130" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A11)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A11)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D11" s="88"/>
-      <c r="E11" s="89" t="str">
+      <c r="D11" s="98"/>
+      <c r="E11" s="131" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A11)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A11)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A11)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F11" s="90"/>
+      <c r="F11" s="86"/>
       <c r="G11" s="35" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A11)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A11)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -2884,12 +2945,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A11)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A11)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L11" s="147" t="str">
+      <c r="L11" s="72" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A11)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A11)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A11)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A11)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A11)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M11" s="148"/>
-      <c r="N11" s="149"/>
+      <c r="M11" s="73"/>
+      <c r="N11" s="74"/>
       <c r="O11" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A11)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A11)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -2926,11 +2987,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A13)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A13)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F12" s="101" t="str">
+      <c r="F12" s="126" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A13)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A13)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G12" s="102"/>
+      <c r="G12" s="84"/>
       <c r="H12" s="39"/>
       <c r="I12" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A13)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A13)-ROW($A$7)+2)/2,0))</f>
@@ -2980,16 +3041,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A13)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A13)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C13" s="91" t="str">
+      <c r="C13" s="128" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A13)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A13)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D13" s="88"/>
-      <c r="E13" s="92" t="str">
+      <c r="D13" s="98"/>
+      <c r="E13" s="129" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A13)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A13)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A13)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F13" s="90"/>
+      <c r="F13" s="86"/>
       <c r="G13" s="36" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A13)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A13)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3007,12 +3068,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A13)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A13)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L13" s="150" t="str">
+      <c r="L13" s="75" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A13)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A13)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A13)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A13)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A13)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M13" s="151"/>
-      <c r="N13" s="152"/>
+      <c r="M13" s="76"/>
+      <c r="N13" s="77"/>
       <c r="O13" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A13)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A13)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3049,11 +3110,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A15)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A15)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F14" s="103" t="str">
+      <c r="F14" s="127" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A15)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A15)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G14" s="102"/>
+      <c r="G14" s="84"/>
       <c r="H14" s="39"/>
       <c r="I14" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A15)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A15)-ROW($A$7)+2)/2,0))</f>
@@ -3106,16 +3167,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A15)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A15)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C15" s="87" t="str">
+      <c r="C15" s="130" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A15)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A15)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D15" s="88"/>
-      <c r="E15" s="89" t="str">
+      <c r="D15" s="98"/>
+      <c r="E15" s="131" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A15)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A15)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A15)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F15" s="90"/>
+      <c r="F15" s="86"/>
       <c r="G15" s="35" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A15)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A15)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3133,12 +3194,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A15)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A15)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L15" s="147" t="str">
+      <c r="L15" s="72" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A15)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A15)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A15)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A15)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A15)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M15" s="148"/>
-      <c r="N15" s="149"/>
+      <c r="M15" s="73"/>
+      <c r="N15" s="74"/>
       <c r="O15" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A15)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A15)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3179,11 +3240,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A17)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A17)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F16" s="101" t="str">
+      <c r="F16" s="126" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A17)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A17)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G16" s="102"/>
+      <c r="G16" s="84"/>
       <c r="H16" s="39"/>
       <c r="I16" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A17)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A17)-ROW($A$7)+2)/2,0))</f>
@@ -3237,16 +3298,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A17)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A17)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C17" s="91" t="str">
+      <c r="C17" s="128" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A17)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A17)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D17" s="88"/>
-      <c r="E17" s="92" t="str">
+      <c r="D17" s="98"/>
+      <c r="E17" s="129" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A17)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A17)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A17)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F17" s="90"/>
+      <c r="F17" s="86"/>
       <c r="G17" s="36" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A17)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A17)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3264,12 +3325,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A17)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A17)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L17" s="150" t="str">
+      <c r="L17" s="75" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A17)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A17)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A17)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A17)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A17)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M17" s="151"/>
-      <c r="N17" s="152"/>
+      <c r="M17" s="76"/>
+      <c r="N17" s="77"/>
       <c r="O17" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A17)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A17)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3310,11 +3371,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A19)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A19)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F18" s="103" t="str">
+      <c r="F18" s="127" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A19)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A19)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G18" s="102"/>
+      <c r="G18" s="84"/>
       <c r="H18" s="39"/>
       <c r="I18" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A19)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A19)-ROW($A$7)+2)/2,0))</f>
@@ -3364,16 +3425,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A19)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A19)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C19" s="87" t="str">
+      <c r="C19" s="130" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A19)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A19)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D19" s="88"/>
-      <c r="E19" s="89" t="str">
+      <c r="D19" s="98"/>
+      <c r="E19" s="131" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A19)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A19)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A19)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F19" s="90"/>
+      <c r="F19" s="86"/>
       <c r="G19" s="35" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A19)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A19)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3391,12 +3452,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A19)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A19)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L19" s="147" t="str">
+      <c r="L19" s="72" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A19)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A19)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A19)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A19)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A19)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M19" s="148"/>
-      <c r="N19" s="149"/>
+      <c r="M19" s="73"/>
+      <c r="N19" s="74"/>
       <c r="O19" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A19)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A19)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3433,11 +3494,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A21)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A21)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F20" s="101" t="str">
+      <c r="F20" s="126" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A21)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A21)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G20" s="102"/>
+      <c r="G20" s="84"/>
       <c r="H20" s="39"/>
       <c r="I20" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A21)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A21)-ROW($A$7)+2)/2,0))</f>
@@ -3485,16 +3546,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A21)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A21)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C21" s="91" t="str">
+      <c r="C21" s="128" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A21)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A21)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D21" s="88"/>
-      <c r="E21" s="92" t="str">
+      <c r="D21" s="98"/>
+      <c r="E21" s="129" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A21)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A21)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A21)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F21" s="90"/>
+      <c r="F21" s="86"/>
       <c r="G21" s="36" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A21)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A21)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3512,12 +3573,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A21)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A21)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L21" s="150" t="str">
+      <c r="L21" s="75" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A21)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A21)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A21)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A21)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A21)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M21" s="151"/>
-      <c r="N21" s="152"/>
+      <c r="M21" s="76"/>
+      <c r="N21" s="77"/>
       <c r="O21" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A21)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A21)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3552,11 +3613,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A23)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A23)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F22" s="103" t="str">
+      <c r="F22" s="127" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A23)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A23)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G22" s="102"/>
+      <c r="G22" s="84"/>
       <c r="H22" s="39"/>
       <c r="I22" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A23)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A23)-ROW($A$7)+2)/2,0))</f>
@@ -3604,16 +3665,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A23)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A23)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C23" s="87" t="str">
+      <c r="C23" s="130" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A23)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A23)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D23" s="88"/>
-      <c r="E23" s="89" t="str">
+      <c r="D23" s="98"/>
+      <c r="E23" s="131" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A23)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A23)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A23)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F23" s="90"/>
+      <c r="F23" s="86"/>
       <c r="G23" s="35" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A23)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A23)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3631,12 +3692,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A23)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A23)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L23" s="147" t="str">
+      <c r="L23" s="72" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A23)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A23)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A23)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A23)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A23)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M23" s="148"/>
-      <c r="N23" s="149"/>
+      <c r="M23" s="73"/>
+      <c r="N23" s="74"/>
       <c r="O23" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A23)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A23)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3671,11 +3732,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A25)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A25)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F24" s="101" t="str">
+      <c r="F24" s="126" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A25)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A25)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G24" s="102"/>
+      <c r="G24" s="84"/>
       <c r="H24" s="39"/>
       <c r="I24" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A25)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A25)-ROW($A$7)+2)/2,0))</f>
@@ -3723,16 +3784,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A25)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A25)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C25" s="91" t="str">
+      <c r="C25" s="128" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A25)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A25)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D25" s="88"/>
-      <c r="E25" s="92" t="str">
+      <c r="D25" s="98"/>
+      <c r="E25" s="129" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A25)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A25)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A25)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F25" s="90"/>
+      <c r="F25" s="86"/>
       <c r="G25" s="36" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A25)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A25)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3750,12 +3811,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A25)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A25)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L25" s="150" t="str">
+      <c r="L25" s="75" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A25)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A25)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A25)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A25)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A25)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M25" s="151"/>
-      <c r="N25" s="152"/>
+      <c r="M25" s="76"/>
+      <c r="N25" s="77"/>
       <c r="O25" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A25)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A25)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3790,11 +3851,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A27)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A27)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F26" s="103" t="str">
+      <c r="F26" s="127" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A27)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A27)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G26" s="102"/>
+      <c r="G26" s="84"/>
       <c r="H26" s="39"/>
       <c r="I26" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A27)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A27)-ROW($A$7)+2)/2,0))</f>
@@ -3836,16 +3897,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A27)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A27)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C27" s="87" t="str">
+      <c r="C27" s="130" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A27)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A27)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D27" s="88"/>
-      <c r="E27" s="89" t="str">
+      <c r="D27" s="98"/>
+      <c r="E27" s="131" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A27)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A27)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A27)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F27" s="90"/>
+      <c r="F27" s="86"/>
       <c r="G27" s="35" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A27)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A27)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3863,12 +3924,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A27)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A27)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L27" s="147" t="str">
+      <c r="L27" s="72" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A27)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A27)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A27)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A27)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A27)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M27" s="148"/>
-      <c r="N27" s="149"/>
+      <c r="M27" s="73"/>
+      <c r="N27" s="74"/>
       <c r="O27" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A27)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A27)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3900,11 +3961,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A29)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A29)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F28" s="101" t="str">
+      <c r="F28" s="126" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A29)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A29)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G28" s="102"/>
+      <c r="G28" s="84"/>
       <c r="H28" s="39"/>
       <c r="I28" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A29)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A29)-ROW($A$7)+2)/2,0))</f>
@@ -3952,16 +4013,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A29)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A29)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C29" s="91" t="str">
+      <c r="C29" s="128" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A29)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A29)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D29" s="88"/>
-      <c r="E29" s="92" t="str">
+      <c r="D29" s="98"/>
+      <c r="E29" s="129" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A29)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A29)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A29)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F29" s="90"/>
+      <c r="F29" s="86"/>
       <c r="G29" s="36" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A29)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A29)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3979,12 +4040,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A29)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A29)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L29" s="150" t="str">
+      <c r="L29" s="75" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A29)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A29)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A29)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A29)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A29)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M29" s="151"/>
-      <c r="N29" s="152"/>
+      <c r="M29" s="76"/>
+      <c r="N29" s="77"/>
       <c r="O29" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A29)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A29)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4023,11 +4084,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A31)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A31)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F30" s="103" t="str">
+      <c r="F30" s="127" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A31)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A31)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G30" s="102"/>
+      <c r="G30" s="84"/>
       <c r="H30" s="39"/>
       <c r="I30" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A31)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A31)-ROW($A$7)+2)/2,0))</f>
@@ -4077,16 +4138,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A31)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A31)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C31" s="87" t="str">
+      <c r="C31" s="130" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A31)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A31)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D31" s="88"/>
-      <c r="E31" s="89" t="str">
+      <c r="D31" s="98"/>
+      <c r="E31" s="131" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A31)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A31)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A31)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F31" s="90"/>
+      <c r="F31" s="86"/>
       <c r="G31" s="35" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A31)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A31)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4104,12 +4165,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A31)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A31)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L31" s="147" t="str">
+      <c r="L31" s="72" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A31)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A31)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A31)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A31)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A31)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M31" s="148"/>
-      <c r="N31" s="149"/>
+      <c r="M31" s="73"/>
+      <c r="N31" s="74"/>
       <c r="O31" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A31)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A31)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4148,11 +4209,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A33)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A33)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F32" s="101" t="str">
+      <c r="F32" s="126" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A33)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A33)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G32" s="102"/>
+      <c r="G32" s="84"/>
       <c r="H32" s="39"/>
       <c r="I32" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A33)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A33)-ROW($A$7)+2)/2,0))</f>
@@ -4204,16 +4265,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A33)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A33)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C33" s="91" t="str">
+      <c r="C33" s="128" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A33)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A33)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D33" s="88"/>
-      <c r="E33" s="92" t="str">
+      <c r="D33" s="98"/>
+      <c r="E33" s="129" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A33)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A33)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A33)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F33" s="90"/>
+      <c r="F33" s="86"/>
       <c r="G33" s="36" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A33)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A33)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4231,12 +4292,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A33)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A33)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L33" s="150" t="str">
+      <c r="L33" s="75" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A33)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A33)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A33)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A33)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A33)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M33" s="151"/>
-      <c r="N33" s="152"/>
+      <c r="M33" s="76"/>
+      <c r="N33" s="77"/>
       <c r="O33" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A33)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A33)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4275,11 +4336,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A35)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A35)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F34" s="103" t="str">
+      <c r="F34" s="127" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A35)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A35)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G34" s="102"/>
+      <c r="G34" s="84"/>
       <c r="H34" s="39"/>
       <c r="I34" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A35)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A35)-ROW($A$7)+2)/2,0))</f>
@@ -4325,16 +4386,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A35)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A35)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C35" s="87" t="str">
+      <c r="C35" s="130" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A35)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A35)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D35" s="88"/>
-      <c r="E35" s="89" t="str">
+      <c r="D35" s="98"/>
+      <c r="E35" s="131" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A35)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A35)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A35)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F35" s="90"/>
+      <c r="F35" s="86"/>
       <c r="G35" s="35" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A35)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A35)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4352,12 +4413,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A35)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A35)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L35" s="147" t="str">
+      <c r="L35" s="72" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A35)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A35)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A35)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A35)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A35)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M35" s="148"/>
-      <c r="N35" s="149"/>
+      <c r="M35" s="73"/>
+      <c r="N35" s="74"/>
       <c r="O35" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A35)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A35)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4390,11 +4451,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A37)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A37)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F36" s="101" t="str">
+      <c r="F36" s="126" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A37)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A37)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G36" s="102"/>
+      <c r="G36" s="84"/>
       <c r="H36" s="39"/>
       <c r="I36" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A37)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A37)-ROW($A$7)+2)/2,0))</f>
@@ -4440,16 +4501,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A37)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A37)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C37" s="91" t="str">
+      <c r="C37" s="128" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A37)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A37)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D37" s="88"/>
-      <c r="E37" s="92" t="str">
+      <c r="D37" s="98"/>
+      <c r="E37" s="129" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A37)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A37)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A37)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F37" s="90"/>
+      <c r="F37" s="86"/>
       <c r="G37" s="36" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A37)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A37)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4467,12 +4528,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A37)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A37)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L37" s="150" t="str">
+      <c r="L37" s="75" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A37)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A37)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A37)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A37)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A37)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M37" s="151"/>
-      <c r="N37" s="152"/>
+      <c r="M37" s="76"/>
+      <c r="N37" s="77"/>
       <c r="O37" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A37)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A37)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4485,15 +4546,15 @@
       <c r="U37" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="V37" s="113" t="s">
+      <c r="V37" s="123" t="s">
         <v>99</v>
       </c>
-      <c r="W37" s="114"/>
-      <c r="X37" s="114"/>
-      <c r="Y37" s="114"/>
-      <c r="Z37" s="114"/>
-      <c r="AA37" s="114"/>
-      <c r="AB37" s="115"/>
+      <c r="W37" s="124"/>
+      <c r="X37" s="124"/>
+      <c r="Y37" s="124"/>
+      <c r="Z37" s="124"/>
+      <c r="AA37" s="124"/>
+      <c r="AB37" s="125"/>
     </row>
     <row r="38" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="31" t="str">
@@ -4516,11 +4577,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A39)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A39)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F38" s="103" t="str">
+      <c r="F38" s="127" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A39)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A39)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G38" s="102"/>
+      <c r="G38" s="84"/>
       <c r="H38" s="39"/>
       <c r="I38" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A39)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A39)-ROW($A$7)+2)/2,0))</f>
@@ -4556,13 +4617,13 @@
       <c r="S38" s="26"/>
       <c r="T38" s="26"/>
       <c r="U38" s="26"/>
-      <c r="V38" s="104"/>
-      <c r="W38" s="105"/>
-      <c r="X38" s="105"/>
-      <c r="Y38" s="105"/>
-      <c r="Z38" s="105"/>
-      <c r="AA38" s="105"/>
-      <c r="AB38" s="106"/>
+      <c r="V38" s="115"/>
+      <c r="W38" s="116"/>
+      <c r="X38" s="116"/>
+      <c r="Y38" s="116"/>
+      <c r="Z38" s="116"/>
+      <c r="AA38" s="116"/>
+      <c r="AB38" s="92"/>
     </row>
     <row r="39" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="str">
@@ -4573,16 +4634,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A39)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A39)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C39" s="87" t="str">
+      <c r="C39" s="130" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A39)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A39)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D39" s="88"/>
-      <c r="E39" s="89" t="str">
+      <c r="D39" s="98"/>
+      <c r="E39" s="131" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A39)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A39)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A39)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F39" s="90"/>
+      <c r="F39" s="86"/>
       <c r="G39" s="35" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A39)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A39)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4600,12 +4661,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A39)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A39)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L39" s="147" t="str">
+      <c r="L39" s="72" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A39)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A39)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A39)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A39)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A39)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M39" s="148"/>
-      <c r="N39" s="149"/>
+      <c r="M39" s="73"/>
+      <c r="N39" s="74"/>
       <c r="O39" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A39)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A39)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4616,13 +4677,13 @@
       <c r="S39" s="26"/>
       <c r="T39" s="26"/>
       <c r="U39" s="26"/>
-      <c r="V39" s="107"/>
-      <c r="W39" s="108"/>
-      <c r="X39" s="108"/>
-      <c r="Y39" s="108"/>
-      <c r="Z39" s="108"/>
-      <c r="AA39" s="108"/>
-      <c r="AB39" s="109"/>
+      <c r="V39" s="117"/>
+      <c r="W39" s="118"/>
+      <c r="X39" s="118"/>
+      <c r="Y39" s="118"/>
+      <c r="Z39" s="118"/>
+      <c r="AA39" s="118"/>
+      <c r="AB39" s="119"/>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" s="33" t="str">
@@ -4645,11 +4706,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A41)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A41)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F40" s="101" t="str">
+      <c r="F40" s="126" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A41)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A41)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G40" s="102"/>
+      <c r="G40" s="84"/>
       <c r="H40" s="39"/>
       <c r="I40" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A41)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A41)-ROW($A$7)+2)/2,0))</f>
@@ -4685,13 +4746,13 @@
       <c r="S40" s="26"/>
       <c r="T40" s="26"/>
       <c r="U40" s="26"/>
-      <c r="V40" s="107"/>
-      <c r="W40" s="108"/>
-      <c r="X40" s="108"/>
-      <c r="Y40" s="108"/>
-      <c r="Z40" s="108"/>
-      <c r="AA40" s="108"/>
-      <c r="AB40" s="109"/>
+      <c r="V40" s="117"/>
+      <c r="W40" s="118"/>
+      <c r="X40" s="118"/>
+      <c r="Y40" s="118"/>
+      <c r="Z40" s="118"/>
+      <c r="AA40" s="118"/>
+      <c r="AB40" s="119"/>
     </row>
     <row r="41" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="19" t="str">
@@ -4702,16 +4763,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A41)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A41)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C41" s="91" t="str">
+      <c r="C41" s="128" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A41)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A41)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D41" s="88"/>
-      <c r="E41" s="92" t="str">
+      <c r="D41" s="98"/>
+      <c r="E41" s="129" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A41)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A41)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A41)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F41" s="90"/>
+      <c r="F41" s="86"/>
       <c r="G41" s="36" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A41)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A41)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4729,12 +4790,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A41)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A41)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L41" s="150" t="str">
+      <c r="L41" s="75" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A41)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A41)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A41)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A41)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A41)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M41" s="151"/>
-      <c r="N41" s="152"/>
+      <c r="M41" s="76"/>
+      <c r="N41" s="77"/>
       <c r="O41" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A41)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A41)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4745,13 +4806,13 @@
       <c r="S41" s="26"/>
       <c r="T41" s="26"/>
       <c r="U41" s="26"/>
-      <c r="V41" s="107"/>
-      <c r="W41" s="108"/>
-      <c r="X41" s="108"/>
-      <c r="Y41" s="108"/>
-      <c r="Z41" s="108"/>
-      <c r="AA41" s="108"/>
-      <c r="AB41" s="109"/>
+      <c r="V41" s="117"/>
+      <c r="W41" s="118"/>
+      <c r="X41" s="118"/>
+      <c r="Y41" s="118"/>
+      <c r="Z41" s="118"/>
+      <c r="AA41" s="118"/>
+      <c r="AB41" s="119"/>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="str">
@@ -4774,11 +4835,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A43)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A43)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F42" s="103" t="str">
+      <c r="F42" s="127" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A43)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A43)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G42" s="102"/>
+      <c r="G42" s="84"/>
       <c r="H42" s="39"/>
       <c r="I42" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A43)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A43)-ROW($A$7)+2)/2,0))</f>
@@ -4814,13 +4875,13 @@
       <c r="S42" s="26"/>
       <c r="T42" s="26"/>
       <c r="U42" s="26"/>
-      <c r="V42" s="107"/>
-      <c r="W42" s="108"/>
-      <c r="X42" s="108"/>
-      <c r="Y42" s="108"/>
-      <c r="Z42" s="108"/>
-      <c r="AA42" s="108"/>
-      <c r="AB42" s="109"/>
+      <c r="V42" s="117"/>
+      <c r="W42" s="118"/>
+      <c r="X42" s="118"/>
+      <c r="Y42" s="118"/>
+      <c r="Z42" s="118"/>
+      <c r="AA42" s="118"/>
+      <c r="AB42" s="119"/>
     </row>
     <row r="43" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="str">
@@ -4831,16 +4892,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A43)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A43)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C43" s="87" t="str">
+      <c r="C43" s="130" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A43)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A43)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D43" s="88"/>
-      <c r="E43" s="89" t="str">
+      <c r="D43" s="98"/>
+      <c r="E43" s="131" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A43)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A43)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A43)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F43" s="90"/>
+      <c r="F43" s="86"/>
       <c r="G43" s="35" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A43)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A43)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4858,12 +4919,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A43)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A43)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L43" s="147" t="str">
+      <c r="L43" s="72" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A43)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A43)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A43)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A43)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A43)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M43" s="148"/>
-      <c r="N43" s="149"/>
+      <c r="M43" s="73"/>
+      <c r="N43" s="74"/>
       <c r="O43" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A43)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A43)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4874,13 +4935,13 @@
       <c r="S43" s="26"/>
       <c r="T43" s="26"/>
       <c r="U43" s="26"/>
-      <c r="V43" s="107"/>
-      <c r="W43" s="108"/>
-      <c r="X43" s="108"/>
-      <c r="Y43" s="108"/>
-      <c r="Z43" s="108"/>
-      <c r="AA43" s="108"/>
-      <c r="AB43" s="109"/>
+      <c r="V43" s="117"/>
+      <c r="W43" s="118"/>
+      <c r="X43" s="118"/>
+      <c r="Y43" s="118"/>
+      <c r="Z43" s="118"/>
+      <c r="AA43" s="118"/>
+      <c r="AB43" s="119"/>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44" s="33" t="str">
@@ -4903,11 +4964,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A45)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A45)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F44" s="101" t="str">
+      <c r="F44" s="126" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A45)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A45)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G44" s="102"/>
+      <c r="G44" s="84"/>
       <c r="H44" s="39"/>
       <c r="I44" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A45)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A45)-ROW($A$7)+2)/2,0))</f>
@@ -4943,13 +5004,13 @@
       <c r="S44" s="26"/>
       <c r="T44" s="26"/>
       <c r="U44" s="26"/>
-      <c r="V44" s="107"/>
-      <c r="W44" s="108"/>
-      <c r="X44" s="108"/>
-      <c r="Y44" s="108"/>
-      <c r="Z44" s="108"/>
-      <c r="AA44" s="108"/>
-      <c r="AB44" s="109"/>
+      <c r="V44" s="117"/>
+      <c r="W44" s="118"/>
+      <c r="X44" s="118"/>
+      <c r="Y44" s="118"/>
+      <c r="Z44" s="118"/>
+      <c r="AA44" s="118"/>
+      <c r="AB44" s="119"/>
     </row>
     <row r="45" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="19" t="str">
@@ -4960,16 +5021,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A45)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A45)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C45" s="91" t="str">
+      <c r="C45" s="128" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A45)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A45)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D45" s="88"/>
-      <c r="E45" s="92" t="str">
+      <c r="D45" s="98"/>
+      <c r="E45" s="129" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A45)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A45)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A45)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F45" s="90"/>
+      <c r="F45" s="86"/>
       <c r="G45" s="36" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A45)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A45)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4987,12 +5048,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A45)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A45)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L45" s="150" t="str">
+      <c r="L45" s="75" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A45)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A45)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A45)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A45)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A45)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M45" s="151"/>
-      <c r="N45" s="152"/>
+      <c r="M45" s="76"/>
+      <c r="N45" s="77"/>
       <c r="O45" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A45)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A45)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5003,13 +5064,13 @@
       <c r="S45" s="26"/>
       <c r="T45" s="26"/>
       <c r="U45" s="26"/>
-      <c r="V45" s="107"/>
-      <c r="W45" s="108"/>
-      <c r="X45" s="108"/>
-      <c r="Y45" s="108"/>
-      <c r="Z45" s="108"/>
-      <c r="AA45" s="108"/>
-      <c r="AB45" s="109"/>
+      <c r="V45" s="117"/>
+      <c r="W45" s="118"/>
+      <c r="X45" s="118"/>
+      <c r="Y45" s="118"/>
+      <c r="Z45" s="118"/>
+      <c r="AA45" s="118"/>
+      <c r="AB45" s="119"/>
     </row>
     <row r="46" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="31" t="str">
@@ -5032,11 +5093,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A47)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A47)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F46" s="103" t="str">
+      <c r="F46" s="127" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A47)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A47)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G46" s="102"/>
+      <c r="G46" s="84"/>
       <c r="H46" s="39"/>
       <c r="I46" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A47)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A47)-ROW($A$7)+2)/2,0))</f>
@@ -5072,13 +5133,13 @@
       <c r="S46" s="26"/>
       <c r="T46" s="26"/>
       <c r="U46" s="26"/>
-      <c r="V46" s="107"/>
-      <c r="W46" s="108"/>
-      <c r="X46" s="108"/>
-      <c r="Y46" s="108"/>
-      <c r="Z46" s="108"/>
-      <c r="AA46" s="108"/>
-      <c r="AB46" s="109"/>
+      <c r="V46" s="117"/>
+      <c r="W46" s="118"/>
+      <c r="X46" s="118"/>
+      <c r="Y46" s="118"/>
+      <c r="Z46" s="118"/>
+      <c r="AA46" s="118"/>
+      <c r="AB46" s="119"/>
     </row>
     <row r="47" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="14" t="str">
@@ -5089,16 +5150,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A47)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A47)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C47" s="87" t="str">
+      <c r="C47" s="130" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A47)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A47)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D47" s="88"/>
-      <c r="E47" s="89" t="str">
+      <c r="D47" s="98"/>
+      <c r="E47" s="131" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A47)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A47)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A47)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F47" s="90"/>
+      <c r="F47" s="86"/>
       <c r="G47" s="35" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A47)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A47)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5116,12 +5177,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A47)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A47)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L47" s="147" t="str">
+      <c r="L47" s="72" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A47)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A47)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A47)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A47)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A47)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M47" s="148"/>
-      <c r="N47" s="149"/>
+      <c r="M47" s="73"/>
+      <c r="N47" s="74"/>
       <c r="O47" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A47)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A47)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5132,13 +5193,13 @@
       <c r="S47" s="26"/>
       <c r="T47" s="26"/>
       <c r="U47" s="26"/>
-      <c r="V47" s="107"/>
-      <c r="W47" s="108"/>
-      <c r="X47" s="108"/>
-      <c r="Y47" s="108"/>
-      <c r="Z47" s="108"/>
-      <c r="AA47" s="108"/>
-      <c r="AB47" s="109"/>
+      <c r="V47" s="117"/>
+      <c r="W47" s="118"/>
+      <c r="X47" s="118"/>
+      <c r="Y47" s="118"/>
+      <c r="Z47" s="118"/>
+      <c r="AA47" s="118"/>
+      <c r="AB47" s="119"/>
     </row>
     <row r="48" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="str">
@@ -5161,11 +5222,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A49)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A49)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F48" s="101" t="str">
+      <c r="F48" s="126" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A49)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A49)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G48" s="102"/>
+      <c r="G48" s="84"/>
       <c r="H48" s="39"/>
       <c r="I48" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A49)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A49)-ROW($A$7)+2)/2,0))</f>
@@ -5201,13 +5262,13 @@
       <c r="S48" s="26"/>
       <c r="T48" s="26"/>
       <c r="U48" s="26"/>
-      <c r="V48" s="107"/>
-      <c r="W48" s="108"/>
-      <c r="X48" s="108"/>
-      <c r="Y48" s="108"/>
-      <c r="Z48" s="108"/>
-      <c r="AA48" s="108"/>
-      <c r="AB48" s="109"/>
+      <c r="V48" s="117"/>
+      <c r="W48" s="118"/>
+      <c r="X48" s="118"/>
+      <c r="Y48" s="118"/>
+      <c r="Z48" s="118"/>
+      <c r="AA48" s="118"/>
+      <c r="AB48" s="119"/>
     </row>
     <row r="49" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="19" t="str">
@@ -5218,16 +5279,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A49)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A49)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C49" s="91" t="str">
+      <c r="C49" s="128" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A49)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A49)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D49" s="88"/>
-      <c r="E49" s="92" t="str">
+      <c r="D49" s="98"/>
+      <c r="E49" s="129" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A49)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A49)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A49)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F49" s="90"/>
+      <c r="F49" s="86"/>
       <c r="G49" s="36" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A49)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A49)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5245,12 +5306,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A49)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A49)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L49" s="150" t="str">
+      <c r="L49" s="75" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A49)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A49)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A49)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A49)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A49)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M49" s="151"/>
-      <c r="N49" s="152"/>
+      <c r="M49" s="76"/>
+      <c r="N49" s="77"/>
       <c r="O49" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A49)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A49)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5261,13 +5322,13 @@
       <c r="S49" s="26"/>
       <c r="T49" s="26"/>
       <c r="U49" s="26"/>
-      <c r="V49" s="107"/>
-      <c r="W49" s="108"/>
-      <c r="X49" s="108"/>
-      <c r="Y49" s="108"/>
-      <c r="Z49" s="108"/>
-      <c r="AA49" s="108"/>
-      <c r="AB49" s="109"/>
+      <c r="V49" s="117"/>
+      <c r="W49" s="118"/>
+      <c r="X49" s="118"/>
+      <c r="Y49" s="118"/>
+      <c r="Z49" s="118"/>
+      <c r="AA49" s="118"/>
+      <c r="AB49" s="119"/>
     </row>
     <row r="50" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="31" t="str">
@@ -5290,11 +5351,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A51)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A51)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F50" s="103" t="str">
+      <c r="F50" s="127" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A51)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A51)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G50" s="102"/>
+      <c r="G50" s="84"/>
       <c r="H50" s="39"/>
       <c r="I50" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A51)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A51)-ROW($A$7)+2)/2,0))</f>
@@ -5330,13 +5391,13 @@
       <c r="S50" s="26"/>
       <c r="T50" s="26"/>
       <c r="U50" s="26"/>
-      <c r="V50" s="107"/>
-      <c r="W50" s="108"/>
-      <c r="X50" s="108"/>
-      <c r="Y50" s="108"/>
-      <c r="Z50" s="108"/>
-      <c r="AA50" s="108"/>
-      <c r="AB50" s="109"/>
+      <c r="V50" s="117"/>
+      <c r="W50" s="118"/>
+      <c r="X50" s="118"/>
+      <c r="Y50" s="118"/>
+      <c r="Z50" s="118"/>
+      <c r="AA50" s="118"/>
+      <c r="AB50" s="119"/>
     </row>
     <row r="51" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="14" t="str">
@@ -5347,16 +5408,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A51)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A51)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C51" s="87" t="str">
+      <c r="C51" s="130" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A51)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A51)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D51" s="88"/>
-      <c r="E51" s="89" t="str">
+      <c r="D51" s="98"/>
+      <c r="E51" s="131" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A51)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A51)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A51)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F51" s="90"/>
+      <c r="F51" s="86"/>
       <c r="G51" s="35" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A51)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A51)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5374,12 +5435,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A51)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A51)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L51" s="147" t="str">
+      <c r="L51" s="72" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A51)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A51)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A51)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A51)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A51)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M51" s="148"/>
-      <c r="N51" s="149"/>
+      <c r="M51" s="73"/>
+      <c r="N51" s="74"/>
       <c r="O51" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A51)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A51)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5390,13 +5451,13 @@
       <c r="S51" s="26"/>
       <c r="T51" s="26"/>
       <c r="U51" s="26"/>
-      <c r="V51" s="107"/>
-      <c r="W51" s="108"/>
-      <c r="X51" s="108"/>
-      <c r="Y51" s="108"/>
-      <c r="Z51" s="108"/>
-      <c r="AA51" s="108"/>
-      <c r="AB51" s="109"/>
+      <c r="V51" s="117"/>
+      <c r="W51" s="118"/>
+      <c r="X51" s="118"/>
+      <c r="Y51" s="118"/>
+      <c r="Z51" s="118"/>
+      <c r="AA51" s="118"/>
+      <c r="AB51" s="119"/>
     </row>
     <row r="52" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="33" t="str">
@@ -5419,11 +5480,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A53)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A53)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F52" s="101" t="str">
+      <c r="F52" s="126" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A53)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A53)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G52" s="102"/>
+      <c r="G52" s="84"/>
       <c r="H52" s="39"/>
       <c r="I52" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A53)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A53)-ROW($A$7)+2)/2,0))</f>
@@ -5459,13 +5520,13 @@
       <c r="S52" s="26"/>
       <c r="T52" s="26"/>
       <c r="U52" s="26"/>
-      <c r="V52" s="107"/>
-      <c r="W52" s="108"/>
-      <c r="X52" s="108"/>
-      <c r="Y52" s="108"/>
-      <c r="Z52" s="108"/>
-      <c r="AA52" s="108"/>
-      <c r="AB52" s="109"/>
+      <c r="V52" s="117"/>
+      <c r="W52" s="118"/>
+      <c r="X52" s="118"/>
+      <c r="Y52" s="118"/>
+      <c r="Z52" s="118"/>
+      <c r="AA52" s="118"/>
+      <c r="AB52" s="119"/>
     </row>
     <row r="53" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="19" t="str">
@@ -5476,16 +5537,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A53)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A53)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C53" s="91" t="str">
+      <c r="C53" s="128" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A53)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A53)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D53" s="88"/>
-      <c r="E53" s="92" t="str">
+      <c r="D53" s="98"/>
+      <c r="E53" s="129" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A53)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A53)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A53)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F53" s="90"/>
+      <c r="F53" s="86"/>
       <c r="G53" s="36" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A53)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A53)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5503,12 +5564,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A53)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A53)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L53" s="150" t="str">
+      <c r="L53" s="75" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A53)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A53)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A53)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A53)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A53)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M53" s="151"/>
-      <c r="N53" s="152"/>
+      <c r="M53" s="76"/>
+      <c r="N53" s="77"/>
       <c r="O53" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A53)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A53)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5519,13 +5580,13 @@
       <c r="S53" s="26"/>
       <c r="T53" s="26"/>
       <c r="U53" s="26"/>
-      <c r="V53" s="110"/>
-      <c r="W53" s="111"/>
-      <c r="X53" s="111"/>
-      <c r="Y53" s="111"/>
-      <c r="Z53" s="111"/>
-      <c r="AA53" s="111"/>
-      <c r="AB53" s="112"/>
+      <c r="V53" s="120"/>
+      <c r="W53" s="121"/>
+      <c r="X53" s="121"/>
+      <c r="Y53" s="121"/>
+      <c r="Z53" s="121"/>
+      <c r="AA53" s="121"/>
+      <c r="AB53" s="122"/>
     </row>
     <row r="54" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="31" t="str">
@@ -5548,11 +5609,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A55)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A55)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F54" s="103" t="str">
+      <c r="F54" s="127" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A55)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A55)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G54" s="102"/>
+      <c r="G54" s="84"/>
       <c r="H54" s="39"/>
       <c r="I54" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A55)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A55)-ROW($A$7)+2)/2,0))</f>
@@ -5598,16 +5659,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A55)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A55)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C55" s="87" t="str">
+      <c r="C55" s="130" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A55)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A55)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D55" s="88"/>
-      <c r="E55" s="89" t="str">
+      <c r="D55" s="98"/>
+      <c r="E55" s="131" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A55)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A55)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A55)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F55" s="90"/>
+      <c r="F55" s="86"/>
       <c r="G55" s="35" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A55)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A55)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5625,12 +5686,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A55)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A55)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L55" s="147" t="str">
+      <c r="L55" s="72" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A55)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A55)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A55)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A55)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A55)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M55" s="148"/>
-      <c r="N55" s="149"/>
+      <c r="M55" s="73"/>
+      <c r="N55" s="74"/>
       <c r="O55" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A55)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A55)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5663,11 +5724,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A57)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A57)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F56" s="101" t="str">
+      <c r="F56" s="126" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A57)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A57)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G56" s="102"/>
+      <c r="G56" s="84"/>
       <c r="H56" s="39"/>
       <c r="I56" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A57)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A57)-ROW($A$7)+2)/2,0))</f>
@@ -5713,16 +5774,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A57)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A57)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C57" s="91" t="str">
+      <c r="C57" s="128" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A57)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A57)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D57" s="88"/>
-      <c r="E57" s="92" t="str">
+      <c r="D57" s="98"/>
+      <c r="E57" s="129" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A57)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A57)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A57)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F57" s="90"/>
+      <c r="F57" s="86"/>
       <c r="G57" s="36" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A57)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A57)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5740,12 +5801,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A57)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A57)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L57" s="150" t="str">
+      <c r="L57" s="75" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A57)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A57)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A57)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A57)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A57)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M57" s="151"/>
-      <c r="N57" s="152"/>
+      <c r="M57" s="76"/>
+      <c r="N57" s="77"/>
       <c r="O57" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A57)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A57)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5778,11 +5839,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A59)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A59)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F58" s="103" t="str">
+      <c r="F58" s="127" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A59)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A59)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G58" s="102"/>
+      <c r="G58" s="84"/>
       <c r="H58" s="39"/>
       <c r="I58" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A59)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A59)-ROW($A$7)+2)/2,0))</f>
@@ -5828,16 +5889,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A59)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A59)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C59" s="87" t="str">
+      <c r="C59" s="130" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A59)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A59)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D59" s="88"/>
-      <c r="E59" s="89" t="str">
+      <c r="D59" s="98"/>
+      <c r="E59" s="131" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A59)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A59)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A59)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F59" s="90"/>
+      <c r="F59" s="86"/>
       <c r="G59" s="35" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A59)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A59)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5855,12 +5916,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A59)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A59)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L59" s="147" t="str">
+      <c r="L59" s="72" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A59)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A59)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A59)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A59)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A59)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M59" s="148"/>
-      <c r="N59" s="149"/>
+      <c r="M59" s="73"/>
+      <c r="N59" s="74"/>
       <c r="O59" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A59)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A59)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5893,11 +5954,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A61)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A61)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F60" s="101" t="str">
+      <c r="F60" s="126" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A61)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A61)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G60" s="102"/>
+      <c r="G60" s="84"/>
       <c r="H60" s="39"/>
       <c r="I60" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A61)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A61)-ROW($A$7)+2)/2,0))</f>
@@ -5943,16 +6004,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A61)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A61)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C61" s="91" t="str">
+      <c r="C61" s="128" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A61)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A61)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D61" s="88"/>
-      <c r="E61" s="92" t="str">
+      <c r="D61" s="98"/>
+      <c r="E61" s="129" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A61)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A61)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A61)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F61" s="90"/>
+      <c r="F61" s="86"/>
       <c r="G61" s="36" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A61)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A61)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5970,12 +6031,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A61)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A61)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L61" s="150" t="str">
+      <c r="L61" s="75" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A61)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A61)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A61)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A61)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A61)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M61" s="151"/>
-      <c r="N61" s="152"/>
+      <c r="M61" s="76"/>
+      <c r="N61" s="77"/>
       <c r="O61" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A61)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A61)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -6008,11 +6069,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A63)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A63)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F62" s="103" t="str">
+      <c r="F62" s="127" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A63)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A63)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G62" s="102"/>
+      <c r="G62" s="84"/>
       <c r="H62" s="39"/>
       <c r="I62" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A63)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A63)-ROW($A$7)+2)/2,0))</f>
@@ -6058,16 +6119,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A63)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A63)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C63" s="87" t="str">
+      <c r="C63" s="130" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A63)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A63)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D63" s="88"/>
-      <c r="E63" s="89" t="str">
+      <c r="D63" s="98"/>
+      <c r="E63" s="131" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A63)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A63)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A63)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F63" s="90"/>
+      <c r="F63" s="86"/>
       <c r="G63" s="35" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A63)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A63)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -6085,12 +6146,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A63)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A63)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L63" s="147" t="str">
+      <c r="L63" s="72" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A63)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A63)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A63)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A63)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A63)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M63" s="148"/>
-      <c r="N63" s="149"/>
+      <c r="M63" s="73"/>
+      <c r="N63" s="74"/>
       <c r="O63" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A63)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A63)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -6123,11 +6184,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A65)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A65)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F64" s="101" t="str">
+      <c r="F64" s="126" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A65)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A65)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G64" s="102"/>
+      <c r="G64" s="84"/>
       <c r="H64" s="39"/>
       <c r="I64" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A65)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A65)-ROW($A$7)+2)/2,0))</f>
@@ -6173,16 +6234,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A65)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A65)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C65" s="91" t="str">
+      <c r="C65" s="128" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A65)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A65)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D65" s="88"/>
-      <c r="E65" s="92" t="str">
+      <c r="D65" s="98"/>
+      <c r="E65" s="129" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A65)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A65)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A65)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F65" s="90"/>
+      <c r="F65" s="86"/>
       <c r="G65" s="36" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A65)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A65)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -6200,12 +6261,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A65)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A65)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L65" s="150" t="str">
+      <c r="L65" s="75" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A65)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A65)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A65)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A65)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A65)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M65" s="151"/>
-      <c r="N65" s="152"/>
+      <c r="M65" s="76"/>
+      <c r="N65" s="77"/>
       <c r="O65" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A65)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A65)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -6238,11 +6299,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A67)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A67)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F66" s="103" t="str">
+      <c r="F66" s="127" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A67)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A67)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G66" s="102"/>
+      <c r="G66" s="84"/>
       <c r="H66" s="39"/>
       <c r="I66" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A67)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A67)-ROW($A$7)+2)/2,0))</f>
@@ -6288,16 +6349,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A67)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A67)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C67" s="87" t="str">
+      <c r="C67" s="130" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A67)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A67)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D67" s="88"/>
-      <c r="E67" s="89" t="str">
+      <c r="D67" s="98"/>
+      <c r="E67" s="131" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A67)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A67)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A67)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F67" s="90"/>
+      <c r="F67" s="86"/>
       <c r="G67" s="35" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A67)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A67)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -6315,12 +6376,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A67)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A67)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L67" s="147" t="str">
+      <c r="L67" s="72" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A67)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A67)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A67)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A67)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A67)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M67" s="148"/>
-      <c r="N67" s="149"/>
+      <c r="M67" s="73"/>
+      <c r="N67" s="74"/>
       <c r="O67" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A67)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A67)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -6353,11 +6414,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A69)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A69)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F68" s="101" t="str">
+      <c r="F68" s="126" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A69)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A69)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G68" s="102"/>
+      <c r="G68" s="84"/>
       <c r="H68" s="39"/>
       <c r="I68" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A69)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A69)-ROW($A$7)+2)/2,0))</f>
@@ -6403,16 +6464,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A69)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A69)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C69" s="91" t="str">
+      <c r="C69" s="128" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A69)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A69)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D69" s="88"/>
-      <c r="E69" s="92" t="str">
+      <c r="D69" s="98"/>
+      <c r="E69" s="129" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A69)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A69)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A69)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F69" s="90"/>
+      <c r="F69" s="86"/>
       <c r="G69" s="36" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A69)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A69)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -6430,12 +6491,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A69)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A69)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L69" s="150" t="str">
+      <c r="L69" s="75" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A69)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A69)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A69)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A69)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A69)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M69" s="151"/>
-      <c r="N69" s="152"/>
+      <c r="M69" s="76"/>
+      <c r="N69" s="77"/>
       <c r="O69" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A69)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A69)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -6468,11 +6529,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A71)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A71)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F70" s="103" t="str">
+      <c r="F70" s="127" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A71)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A71)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G70" s="102"/>
+      <c r="G70" s="84"/>
       <c r="H70" s="39"/>
       <c r="I70" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A71)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A71)-ROW($A$7)+2)/2,0))</f>
@@ -6518,16 +6579,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A71)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A71)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C71" s="87" t="str">
+      <c r="C71" s="130" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A71)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A71)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D71" s="88"/>
-      <c r="E71" s="89" t="str">
+      <c r="D71" s="98"/>
+      <c r="E71" s="131" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A71)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A71)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A71)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F71" s="90"/>
+      <c r="F71" s="86"/>
       <c r="G71" s="35" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A71)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A71)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -6545,12 +6606,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A71)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A71)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L71" s="147" t="str">
+      <c r="L71" s="72" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A71)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A71)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A71)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A71)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A71)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M71" s="148"/>
-      <c r="N71" s="149"/>
+      <c r="M71" s="73"/>
+      <c r="N71" s="74"/>
       <c r="O71" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A71)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A71)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -6563,377 +6624,448 @@
       <c r="U71" s="26"/>
     </row>
     <row r="72" spans="1:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="93" t="s">
+      <c r="A72" s="132" t="s">
         <v>100</v>
       </c>
-      <c r="B72" s="94"/>
-      <c r="C72" s="94"/>
-      <c r="D72" s="94"/>
-      <c r="E72" s="94"/>
-      <c r="F72" s="94"/>
-      <c r="G72" s="94"/>
-      <c r="H72" s="94"/>
-      <c r="I72" s="94"/>
-      <c r="J72" s="94"/>
-      <c r="K72" s="94"/>
-      <c r="L72" s="94"/>
-      <c r="M72" s="94"/>
-      <c r="N72" s="94"/>
-      <c r="O72" s="95"/>
+      <c r="B72" s="133"/>
+      <c r="C72" s="133"/>
+      <c r="D72" s="133"/>
+      <c r="E72" s="133"/>
+      <c r="F72" s="133"/>
+      <c r="G72" s="133"/>
+      <c r="H72" s="133"/>
+      <c r="I72" s="133"/>
+      <c r="J72" s="133"/>
+      <c r="K72" s="133"/>
+      <c r="L72" s="133"/>
+      <c r="M72" s="133"/>
+      <c r="N72" s="133"/>
+      <c r="O72" s="134"/>
       <c r="S72" s="26"/>
       <c r="T72" s="26"/>
     </row>
     <row r="73" spans="1:21" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="96"/>
-      <c r="B73" s="97"/>
-      <c r="C73" s="97"/>
-      <c r="D73" s="97"/>
-      <c r="E73" s="97"/>
-      <c r="F73" s="97"/>
-      <c r="G73" s="97"/>
-      <c r="H73" s="97"/>
-      <c r="I73" s="97"/>
-      <c r="J73" s="97"/>
-      <c r="K73" s="97"/>
-      <c r="L73" s="97"/>
-      <c r="M73" s="97"/>
-      <c r="N73" s="97"/>
-      <c r="O73" s="98"/>
+      <c r="A73" s="135"/>
+      <c r="B73" s="136"/>
+      <c r="C73" s="136"/>
+      <c r="D73" s="136"/>
+      <c r="E73" s="136"/>
+      <c r="F73" s="136"/>
+      <c r="G73" s="136"/>
+      <c r="H73" s="136"/>
+      <c r="I73" s="136"/>
+      <c r="J73" s="136"/>
+      <c r="K73" s="136"/>
+      <c r="L73" s="136"/>
+      <c r="M73" s="136"/>
+      <c r="N73" s="136"/>
+      <c r="O73" s="137"/>
       <c r="S73" s="26"/>
       <c r="T73" s="26"/>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A74" s="81" t="s">
+      <c r="A74" s="138" t="s">
         <v>101</v>
       </c>
-      <c r="B74" s="76"/>
-      <c r="C74" s="77"/>
-      <c r="D74" s="77"/>
-      <c r="E74" s="77"/>
-      <c r="F74" s="77"/>
-      <c r="G74" s="70"/>
+      <c r="B74" s="140"/>
+      <c r="C74" s="141"/>
+      <c r="D74" s="141"/>
+      <c r="E74" s="141"/>
+      <c r="F74" s="141"/>
+      <c r="G74" s="142"/>
       <c r="H74" s="68"/>
-      <c r="I74" s="99" t="s">
+      <c r="I74" s="146" t="s">
         <v>105</v>
       </c>
-      <c r="J74" s="76"/>
-      <c r="K74" s="77"/>
-      <c r="L74" s="77"/>
-      <c r="M74" s="77"/>
-      <c r="N74" s="77"/>
-      <c r="O74" s="70"/>
+      <c r="J74" s="140"/>
+      <c r="K74" s="141"/>
+      <c r="L74" s="141"/>
+      <c r="M74" s="141"/>
+      <c r="N74" s="141"/>
+      <c r="O74" s="142"/>
     </row>
     <row r="75" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="82"/>
-      <c r="B75" s="76"/>
-      <c r="C75" s="77"/>
-      <c r="D75" s="77"/>
-      <c r="E75" s="77"/>
-      <c r="F75" s="77"/>
-      <c r="G75" s="70"/>
+      <c r="A75" s="139"/>
+      <c r="B75" s="140"/>
+      <c r="C75" s="141"/>
+      <c r="D75" s="141"/>
+      <c r="E75" s="141"/>
+      <c r="F75" s="141"/>
+      <c r="G75" s="142"/>
       <c r="H75" s="56"/>
-      <c r="I75" s="82"/>
-      <c r="J75" s="76"/>
-      <c r="K75" s="77"/>
-      <c r="L75" s="77"/>
-      <c r="M75" s="77"/>
-      <c r="N75" s="77"/>
-      <c r="O75" s="70"/>
+      <c r="I75" s="139"/>
+      <c r="J75" s="140"/>
+      <c r="K75" s="141"/>
+      <c r="L75" s="141"/>
+      <c r="M75" s="141"/>
+      <c r="N75" s="141"/>
+      <c r="O75" s="142"/>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A76" s="84"/>
-      <c r="B76" s="76"/>
-      <c r="C76" s="77"/>
-      <c r="D76" s="77"/>
-      <c r="E76" s="77"/>
-      <c r="F76" s="77"/>
-      <c r="G76" s="70"/>
+      <c r="A76" s="147"/>
+      <c r="B76" s="140"/>
+      <c r="C76" s="141"/>
+      <c r="D76" s="141"/>
+      <c r="E76" s="141"/>
+      <c r="F76" s="141"/>
+      <c r="G76" s="142"/>
       <c r="H76" s="68"/>
-      <c r="I76" s="70"/>
-      <c r="J76" s="76"/>
-      <c r="K76" s="77"/>
-      <c r="L76" s="77"/>
-      <c r="M76" s="77"/>
-      <c r="N76" s="77"/>
-      <c r="O76" s="70"/>
-    </row>
-    <row r="77" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="84"/>
-      <c r="B77" s="78"/>
-      <c r="C77" s="79"/>
-      <c r="D77" s="79"/>
-      <c r="E77" s="79"/>
-      <c r="F77" s="79"/>
-      <c r="G77" s="80"/>
+      <c r="I76" s="142"/>
+      <c r="J76" s="140"/>
+      <c r="K76" s="141"/>
+      <c r="L76" s="141"/>
+      <c r="M76" s="141"/>
+      <c r="N76" s="141"/>
+      <c r="O76" s="142"/>
+    </row>
+    <row r="77" spans="1:21" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="147"/>
+      <c r="B77" s="143"/>
+      <c r="C77" s="144"/>
+      <c r="D77" s="144"/>
+      <c r="E77" s="144"/>
+      <c r="F77" s="144"/>
+      <c r="G77" s="145"/>
       <c r="H77" s="68"/>
-      <c r="I77" s="70"/>
-      <c r="J77" s="78"/>
-      <c r="K77" s="79"/>
-      <c r="L77" s="79"/>
-      <c r="M77" s="79"/>
-      <c r="N77" s="79"/>
-      <c r="O77" s="80"/>
+      <c r="I77" s="142"/>
+      <c r="J77" s="143"/>
+      <c r="K77" s="144"/>
+      <c r="L77" s="144"/>
+      <c r="M77" s="144"/>
+      <c r="N77" s="144"/>
+      <c r="O77" s="145"/>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A78" s="100" t="s">
+      <c r="A78" s="148" t="s">
         <v>102</v>
       </c>
-      <c r="B78" s="73"/>
-      <c r="C78" s="74"/>
-      <c r="D78" s="74"/>
-      <c r="E78" s="74"/>
-      <c r="F78" s="74"/>
-      <c r="G78" s="75"/>
+      <c r="B78" s="149"/>
+      <c r="C78" s="150"/>
+      <c r="D78" s="150"/>
+      <c r="E78" s="150"/>
+      <c r="F78" s="150"/>
+      <c r="G78" s="151"/>
       <c r="H78" s="39"/>
-      <c r="I78" s="81" t="s">
+      <c r="I78" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="J78" s="76"/>
-      <c r="K78" s="77"/>
-      <c r="L78" s="77"/>
-      <c r="M78" s="77"/>
-      <c r="N78" s="77"/>
-      <c r="O78" s="70"/>
+      <c r="J78" s="140"/>
+      <c r="K78" s="141"/>
+      <c r="L78" s="141"/>
+      <c r="M78" s="141"/>
+      <c r="N78" s="141"/>
+      <c r="O78" s="142"/>
     </row>
     <row r="79" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="82"/>
-      <c r="B79" s="76"/>
-      <c r="C79" s="77"/>
-      <c r="D79" s="77"/>
-      <c r="E79" s="77"/>
-      <c r="F79" s="77"/>
-      <c r="G79" s="70"/>
+      <c r="A79" s="139"/>
+      <c r="B79" s="140"/>
+      <c r="C79" s="141"/>
+      <c r="D79" s="141"/>
+      <c r="E79" s="141"/>
+      <c r="F79" s="141"/>
+      <c r="G79" s="142"/>
       <c r="H79" s="56"/>
-      <c r="I79" s="82"/>
-      <c r="J79" s="76"/>
-      <c r="K79" s="77"/>
-      <c r="L79" s="77"/>
-      <c r="M79" s="77"/>
-      <c r="N79" s="77"/>
-      <c r="O79" s="70"/>
+      <c r="I79" s="139"/>
+      <c r="J79" s="140"/>
+      <c r="K79" s="141"/>
+      <c r="L79" s="141"/>
+      <c r="M79" s="141"/>
+      <c r="N79" s="141"/>
+      <c r="O79" s="142"/>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A80" s="84"/>
-      <c r="B80" s="76"/>
-      <c r="C80" s="77"/>
-      <c r="D80" s="77"/>
-      <c r="E80" s="77"/>
-      <c r="F80" s="77"/>
-      <c r="G80" s="70"/>
+      <c r="A80" s="147"/>
+      <c r="B80" s="140"/>
+      <c r="C80" s="141"/>
+      <c r="D80" s="141"/>
+      <c r="E80" s="141"/>
+      <c r="F80" s="141"/>
+      <c r="G80" s="142"/>
       <c r="H80" s="39"/>
-      <c r="I80" s="70"/>
-      <c r="J80" s="76"/>
-      <c r="K80" s="77"/>
-      <c r="L80" s="77"/>
-      <c r="M80" s="77"/>
-      <c r="N80" s="77"/>
-      <c r="O80" s="70"/>
-    </row>
-    <row r="81" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="84"/>
-      <c r="B81" s="78"/>
-      <c r="C81" s="79"/>
-      <c r="D81" s="79"/>
-      <c r="E81" s="79"/>
-      <c r="F81" s="79"/>
-      <c r="G81" s="80"/>
+      <c r="I80" s="142"/>
+      <c r="J80" s="140"/>
+      <c r="K80" s="141"/>
+      <c r="L80" s="141"/>
+      <c r="M80" s="141"/>
+      <c r="N80" s="141"/>
+      <c r="O80" s="142"/>
+    </row>
+    <row r="81" spans="1:15" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="147"/>
+      <c r="B81" s="143"/>
+      <c r="C81" s="144"/>
+      <c r="D81" s="144"/>
+      <c r="E81" s="144"/>
+      <c r="F81" s="144"/>
+      <c r="G81" s="145"/>
       <c r="H81" s="39"/>
-      <c r="I81" s="70"/>
-      <c r="J81" s="78"/>
-      <c r="K81" s="79"/>
-      <c r="L81" s="79"/>
-      <c r="M81" s="79"/>
-      <c r="N81" s="79"/>
-      <c r="O81" s="80"/>
+      <c r="I81" s="142"/>
+      <c r="J81" s="143"/>
+      <c r="K81" s="144"/>
+      <c r="L81" s="144"/>
+      <c r="M81" s="144"/>
+      <c r="N81" s="144"/>
+      <c r="O81" s="145"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A82" s="71" t="s">
+      <c r="A82" s="78" t="s">
         <v>103</v>
       </c>
-      <c r="B82" s="73"/>
-      <c r="C82" s="74"/>
-      <c r="D82" s="74"/>
-      <c r="E82" s="74"/>
-      <c r="F82" s="74"/>
-      <c r="G82" s="75"/>
+      <c r="B82" s="149"/>
+      <c r="C82" s="150"/>
+      <c r="D82" s="150"/>
+      <c r="E82" s="150"/>
+      <c r="F82" s="150"/>
+      <c r="G82" s="151"/>
       <c r="H82" s="39"/>
-      <c r="I82" s="81" t="s">
+      <c r="I82" s="138" t="s">
         <v>107</v>
       </c>
-      <c r="J82" s="76"/>
-      <c r="K82" s="77"/>
-      <c r="L82" s="77"/>
-      <c r="M82" s="77"/>
-      <c r="N82" s="77"/>
-      <c r="O82" s="70"/>
+      <c r="J82" s="140"/>
+      <c r="K82" s="141"/>
+      <c r="L82" s="141"/>
+      <c r="M82" s="141"/>
+      <c r="N82" s="141"/>
+      <c r="O82" s="142"/>
     </row>
     <row r="83" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="72"/>
-      <c r="B83" s="76"/>
-      <c r="C83" s="77"/>
-      <c r="D83" s="77"/>
-      <c r="E83" s="77"/>
-      <c r="F83" s="77"/>
-      <c r="G83" s="70"/>
+      <c r="A83" s="153"/>
+      <c r="B83" s="140"/>
+      <c r="C83" s="141"/>
+      <c r="D83" s="141"/>
+      <c r="E83" s="141"/>
+      <c r="F83" s="141"/>
+      <c r="G83" s="142"/>
       <c r="H83" s="56"/>
-      <c r="I83" s="82"/>
-      <c r="J83" s="76"/>
-      <c r="K83" s="77"/>
-      <c r="L83" s="77"/>
-      <c r="M83" s="77"/>
-      <c r="N83" s="77"/>
-      <c r="O83" s="70"/>
+      <c r="I83" s="139"/>
+      <c r="J83" s="140"/>
+      <c r="K83" s="141"/>
+      <c r="L83" s="141"/>
+      <c r="M83" s="141"/>
+      <c r="N83" s="141"/>
+      <c r="O83" s="142"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A84" s="83"/>
-      <c r="B84" s="76"/>
-      <c r="C84" s="77"/>
-      <c r="D84" s="77"/>
-      <c r="E84" s="77"/>
-      <c r="F84" s="77"/>
-      <c r="G84" s="70"/>
+      <c r="A84" s="154"/>
+      <c r="B84" s="140"/>
+      <c r="C84" s="141"/>
+      <c r="D84" s="141"/>
+      <c r="E84" s="141"/>
+      <c r="F84" s="141"/>
+      <c r="G84" s="142"/>
       <c r="H84" s="39"/>
-      <c r="I84" s="70"/>
-      <c r="J84" s="76"/>
-      <c r="K84" s="77"/>
-      <c r="L84" s="77"/>
-      <c r="M84" s="77"/>
-      <c r="N84" s="77"/>
-      <c r="O84" s="70"/>
-    </row>
-    <row r="85" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="84"/>
-      <c r="B85" s="78"/>
-      <c r="C85" s="79"/>
-      <c r="D85" s="79"/>
-      <c r="E85" s="79"/>
-      <c r="F85" s="79"/>
-      <c r="G85" s="80"/>
+      <c r="I84" s="142"/>
+      <c r="J84" s="140"/>
+      <c r="K84" s="141"/>
+      <c r="L84" s="141"/>
+      <c r="M84" s="141"/>
+      <c r="N84" s="141"/>
+      <c r="O84" s="142"/>
+    </row>
+    <row r="85" spans="1:15" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="147"/>
+      <c r="B85" s="143"/>
+      <c r="C85" s="144"/>
+      <c r="D85" s="144"/>
+      <c r="E85" s="144"/>
+      <c r="F85" s="144"/>
+      <c r="G85" s="145"/>
       <c r="H85" s="39"/>
-      <c r="I85" s="70"/>
-      <c r="J85" s="78"/>
-      <c r="K85" s="79"/>
-      <c r="L85" s="79"/>
-      <c r="M85" s="79"/>
-      <c r="N85" s="79"/>
-      <c r="O85" s="80"/>
+      <c r="I85" s="142"/>
+      <c r="J85" s="143"/>
+      <c r="K85" s="144"/>
+      <c r="L85" s="144"/>
+      <c r="M85" s="144"/>
+      <c r="N85" s="144"/>
+      <c r="O85" s="145"/>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A86" s="71" t="s">
+      <c r="A86" s="78" t="s">
         <v>104</v>
       </c>
-      <c r="B86" s="73"/>
-      <c r="C86" s="74"/>
-      <c r="D86" s="74"/>
-      <c r="E86" s="74"/>
-      <c r="F86" s="74"/>
-      <c r="G86" s="75"/>
+      <c r="B86" s="149"/>
+      <c r="C86" s="150"/>
+      <c r="D86" s="150"/>
+      <c r="E86" s="150"/>
+      <c r="F86" s="150"/>
+      <c r="G86" s="151"/>
       <c r="H86" s="39"/>
-      <c r="I86" s="81" t="s">
+      <c r="I86" s="138" t="s">
         <v>108</v>
       </c>
-      <c r="J86" s="76"/>
-      <c r="K86" s="77"/>
-      <c r="L86" s="77"/>
-      <c r="M86" s="77"/>
-      <c r="N86" s="77"/>
-      <c r="O86" s="70"/>
+      <c r="J86" s="140"/>
+      <c r="K86" s="141"/>
+      <c r="L86" s="141"/>
+      <c r="M86" s="141"/>
+      <c r="N86" s="141"/>
+      <c r="O86" s="142"/>
     </row>
     <row r="87" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="72"/>
-      <c r="B87" s="76"/>
-      <c r="C87" s="77"/>
-      <c r="D87" s="77"/>
-      <c r="E87" s="77"/>
-      <c r="F87" s="77"/>
-      <c r="G87" s="70"/>
+      <c r="A87" s="153"/>
+      <c r="B87" s="140"/>
+      <c r="C87" s="141"/>
+      <c r="D87" s="141"/>
+      <c r="E87" s="141"/>
+      <c r="F87" s="141"/>
+      <c r="G87" s="142"/>
       <c r="H87" s="56"/>
-      <c r="I87" s="82"/>
-      <c r="J87" s="76"/>
-      <c r="K87" s="77"/>
-      <c r="L87" s="77"/>
-      <c r="M87" s="77"/>
-      <c r="N87" s="77"/>
-      <c r="O87" s="70"/>
+      <c r="I87" s="139"/>
+      <c r="J87" s="140"/>
+      <c r="K87" s="141"/>
+      <c r="L87" s="141"/>
+      <c r="M87" s="141"/>
+      <c r="N87" s="141"/>
+      <c r="O87" s="142"/>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A88" s="83"/>
-      <c r="B88" s="76"/>
-      <c r="C88" s="77"/>
-      <c r="D88" s="77"/>
-      <c r="E88" s="77"/>
-      <c r="F88" s="77"/>
-      <c r="G88" s="70"/>
+      <c r="A88" s="154"/>
+      <c r="B88" s="140"/>
+      <c r="C88" s="141"/>
+      <c r="D88" s="141"/>
+      <c r="E88" s="141"/>
+      <c r="F88" s="141"/>
+      <c r="G88" s="142"/>
       <c r="H88" s="39"/>
-      <c r="I88" s="70"/>
-      <c r="J88" s="76"/>
-      <c r="K88" s="77"/>
-      <c r="L88" s="77"/>
-      <c r="M88" s="77"/>
-      <c r="N88" s="77"/>
-      <c r="O88" s="70"/>
-    </row>
-    <row r="89" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="85"/>
-      <c r="B89" s="78"/>
-      <c r="C89" s="79"/>
-      <c r="D89" s="79"/>
-      <c r="E89" s="79"/>
-      <c r="F89" s="79"/>
-      <c r="G89" s="80"/>
+      <c r="I88" s="142"/>
+      <c r="J88" s="140"/>
+      <c r="K88" s="141"/>
+      <c r="L88" s="141"/>
+      <c r="M88" s="141"/>
+      <c r="N88" s="141"/>
+      <c r="O88" s="142"/>
+    </row>
+    <row r="89" spans="1:15" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="155"/>
+      <c r="B89" s="143"/>
+      <c r="C89" s="144"/>
+      <c r="D89" s="144"/>
+      <c r="E89" s="144"/>
+      <c r="F89" s="144"/>
+      <c r="G89" s="145"/>
       <c r="H89" s="69"/>
-      <c r="I89" s="80"/>
-      <c r="J89" s="78"/>
-      <c r="K89" s="79"/>
-      <c r="L89" s="79"/>
-      <c r="M89" s="79"/>
-      <c r="N89" s="79"/>
-      <c r="O89" s="80"/>
+      <c r="I89" s="145"/>
+      <c r="J89" s="143"/>
+      <c r="K89" s="144"/>
+      <c r="L89" s="144"/>
+      <c r="M89" s="144"/>
+      <c r="N89" s="144"/>
+      <c r="O89" s="145"/>
     </row>
   </sheetData>
   <mergeCells count="179">
-    <mergeCell ref="L63:N63"/>
-    <mergeCell ref="L65:N65"/>
-    <mergeCell ref="L67:N67"/>
-    <mergeCell ref="L69:N69"/>
-    <mergeCell ref="L71:N71"/>
-    <mergeCell ref="L45:N45"/>
-    <mergeCell ref="L47:N47"/>
-    <mergeCell ref="L49:N49"/>
-    <mergeCell ref="L51:N51"/>
-    <mergeCell ref="L53:N53"/>
-    <mergeCell ref="L55:N55"/>
-    <mergeCell ref="L57:N57"/>
-    <mergeCell ref="L59:N59"/>
-    <mergeCell ref="L61:N61"/>
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="L29:N29"/>
-    <mergeCell ref="L31:N31"/>
-    <mergeCell ref="L33:N33"/>
-    <mergeCell ref="L35:N35"/>
-    <mergeCell ref="L37:N37"/>
-    <mergeCell ref="L39:N39"/>
-    <mergeCell ref="L41:N41"/>
-    <mergeCell ref="L43:N43"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="B82:G85"/>
+    <mergeCell ref="I82:I83"/>
+    <mergeCell ref="J82:O85"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="I84:I85"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="B86:G89"/>
+    <mergeCell ref="I86:I87"/>
+    <mergeCell ref="J86:O89"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="I88:I89"/>
+    <mergeCell ref="S3:T4"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="A72:O73"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:G77"/>
+    <mergeCell ref="I74:I75"/>
+    <mergeCell ref="J74:O77"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="I76:I77"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="B78:G81"/>
+    <mergeCell ref="I78:I79"/>
+    <mergeCell ref="J78:O81"/>
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="I80:I81"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F18:G18"/>
     <mergeCell ref="V38:AB53"/>
     <mergeCell ref="V37:AB37"/>
     <mergeCell ref="F36:G36"/>
@@ -6958,125 +7090,54 @@
     <mergeCell ref="L21:N21"/>
     <mergeCell ref="L23:N23"/>
     <mergeCell ref="L25:N25"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="A72:O73"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="B74:G77"/>
-    <mergeCell ref="I74:I75"/>
-    <mergeCell ref="J74:O77"/>
-    <mergeCell ref="A76:A77"/>
-    <mergeCell ref="I76:I77"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="B78:G81"/>
-    <mergeCell ref="I78:I79"/>
-    <mergeCell ref="J78:O81"/>
-    <mergeCell ref="A80:A81"/>
-    <mergeCell ref="S3:T4"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="I80:I81"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="B82:G85"/>
-    <mergeCell ref="I82:I83"/>
-    <mergeCell ref="J82:O85"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="I84:I85"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="B86:G89"/>
-    <mergeCell ref="I86:I87"/>
-    <mergeCell ref="J86:O89"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="I88:I89"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="L29:N29"/>
+    <mergeCell ref="L31:N31"/>
+    <mergeCell ref="L33:N33"/>
+    <mergeCell ref="L35:N35"/>
+    <mergeCell ref="L37:N37"/>
+    <mergeCell ref="L39:N39"/>
+    <mergeCell ref="L41:N41"/>
+    <mergeCell ref="L43:N43"/>
+    <mergeCell ref="L63:N63"/>
+    <mergeCell ref="L65:N65"/>
+    <mergeCell ref="L67:N67"/>
+    <mergeCell ref="L69:N69"/>
+    <mergeCell ref="L71:N71"/>
+    <mergeCell ref="L45:N45"/>
+    <mergeCell ref="L47:N47"/>
+    <mergeCell ref="L49:N49"/>
+    <mergeCell ref="L51:N51"/>
+    <mergeCell ref="L53:N53"/>
+    <mergeCell ref="L55:N55"/>
+    <mergeCell ref="L57:N57"/>
+    <mergeCell ref="L59:N59"/>
+    <mergeCell ref="L61:N61"/>
   </mergeCells>
   <conditionalFormatting sqref="O6 O10 O14 O18 O22 O26 O30 O34 O38 O42 O46 O50 O54 O58 O62 O66 O70">
-    <cfRule type="expression" dxfId="12" priority="4">
+    <cfRule type="expression" dxfId="11" priority="4">
       <formula>O6="Unachiev"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>OR(O6="ZONE",O6="LAR")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="10" priority="6">
@@ -7087,10 +7148,10 @@
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>O8="Unachiev"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="2">
-      <formula>O8="ZONE"</formula>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>OR(O8="ZONE",O8="LAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula>O8="RANGE"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7106,13 +7167,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" style="25" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="71" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" style="25" customWidth="1"/>
     <col min="10" max="10" width="12.28515625" style="25" customWidth="1"/>
     <col min="11" max="11" width="10.140625" style="25" customWidth="1"/>
@@ -7146,7 +7206,7 @@
       <c r="G1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="70" t="s">
         <v>114</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -7221,7 +7281,7 @@
       <c r="E2" s="30"/>
       <c r="F2" s="30"/>
       <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
+      <c r="H2" s="71"/>
       <c r="I2" s="67"/>
       <c r="J2" s="67"/>
       <c r="K2" s="67"/>
@@ -7252,7 +7312,7 @@
       <c r="E3" s="30"/>
       <c r="F3" s="30"/>
       <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
+      <c r="H3" s="71"/>
       <c r="I3" s="67"/>
       <c r="J3" s="67"/>
       <c r="K3" s="67"/>
@@ -7283,7 +7343,7 @@
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
       <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
+      <c r="H4" s="71"/>
       <c r="I4" s="67"/>
       <c r="J4" s="67"/>
       <c r="K4" s="67"/>
@@ -7314,7 +7374,6 @@
       <c r="E5" s="67"/>
       <c r="F5" s="30"/>
       <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
       <c r="I5" s="67"/>
       <c r="J5" s="67"/>
       <c r="K5" s="67"/>
@@ -7345,7 +7404,6 @@
       <c r="E6" s="67"/>
       <c r="F6" s="30"/>
       <c r="G6" s="67"/>
-      <c r="H6" s="67"/>
       <c r="I6" s="67"/>
       <c r="J6" s="67"/>
       <c r="K6" s="67"/>

</xml_diff>

<commit_message>
JASSM DT show blank for JDPI ID Changelog and How To Guide split seperately
</commit_message>
<xml_diff>
--- a/Debrief Sheet Template v4.xlsx
+++ b/Debrief Sheet Template v4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Python\bidds-debrief\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED83F4A0-3EC1-4302-AB92-CA8D6A93B6D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC828FC-AA31-4F30-9152-C7D653C087DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22845" yWindow="2670" windowWidth="19950" windowHeight="17235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26895" yWindow="2745" windowWidth="28845" windowHeight="17235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Debrief" sheetId="1" r:id="rId1"/>
@@ -1530,117 +1530,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="8" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
+    <xf numFmtId="165" fontId="5" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="172" fontId="9" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
@@ -1652,140 +1627,111 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="9" fillId="8" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="172" fontId="9" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="26" formatCode="h:mm:ss"/>
     </dxf>
@@ -1865,6 +1811,60 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1884,17 +1884,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="S5:T17" headerRowCount="0" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="S5:T17" headerRowCount="0" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" headerRowDxfId="11" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" headerRowDxfId="9" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" headerRowDxfId="5" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" headerRowDxfId="3" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:AE100" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:AE100" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:AE100" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="31">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Record Number"/>
@@ -1904,7 +1904,7 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="TOT"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="TOR"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="BULL"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="TOF" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="TOF" dataDxfId="0"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="WPN Type"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="TGT Name"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="TGT LAT"/>
@@ -2260,7 +2260,7 @@
   <dimension ref="A1:AB84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23:N23"/>
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2281,107 +2281,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="112" t="str">
+      <c r="A1" s="150" t="str">
         <f>IF(ISBLANK(cs),"",cs)</f>
         <v/>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="114" t="s">
+      <c r="B1" s="151"/>
+      <c r="C1" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="152"/>
       <c r="F1" s="62"/>
       <c r="G1" s="63"/>
       <c r="H1" s="61"/>
-      <c r="I1" s="81" t="s">
+      <c r="I1" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="83"/>
+      <c r="J1" s="124"/>
+      <c r="K1" s="124"/>
+      <c r="L1" s="124"/>
+      <c r="M1" s="124"/>
+      <c r="N1" s="124"/>
+      <c r="O1" s="125"/>
     </row>
     <row r="2" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="98" t="str">
+      <c r="A2" s="137" t="str">
         <f>IF(msndate=0,"",msndate)</f>
         <v/>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="104" t="s">
+      <c r="B2" s="138"/>
+      <c r="C2" s="142" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="105"/>
+      <c r="D2" s="143"/>
       <c r="E2" s="9" t="str">
         <f>IF(ISBLANK(msnlead),"",msnlead)</f>
         <v/>
       </c>
-      <c r="F2" s="94" t="s">
+      <c r="F2" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="95"/>
+      <c r="G2" s="108"/>
       <c r="H2" s="61"/>
-      <c r="I2" s="84" t="s">
+      <c r="I2" s="126" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="85"/>
-      <c r="K2" s="108" t="str">
+      <c r="J2" s="127"/>
+      <c r="K2" s="146" t="str">
         <f>IF(ISBLANK(tgp),"",tgp)</f>
         <v>SNIPER</v>
       </c>
-      <c r="L2" s="85"/>
+      <c r="L2" s="127"/>
       <c r="M2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="86" t="str">
+      <c r="N2" s="128" t="str">
         <f>IF(ISBLANK(dtcsortie),"",dtcsortie)</f>
         <v/>
       </c>
-      <c r="O2" s="87"/>
+      <c r="O2" s="100"/>
     </row>
     <row r="3" spans="1:28" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="100" t="str">
+      <c r="A3" s="139" t="str">
         <f>IF(msnnum=0,"",msnnum)</f>
         <v/>
       </c>
-      <c r="B3" s="101"/>
-      <c r="C3" s="106" t="s">
+      <c r="B3" s="94"/>
+      <c r="C3" s="144" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="107"/>
+      <c r="D3" s="145"/>
       <c r="E3" s="64" t="str">
         <f>IF(ISBLANK(msnwso),"",msnwso)</f>
         <v/>
       </c>
-      <c r="F3" s="92" t="str">
+      <c r="F3" s="132" t="str">
         <f>IF(ISBLANK(Combined!B2),"",Combined!B2)</f>
         <v/>
       </c>
-      <c r="G3" s="93"/>
+      <c r="G3" s="133"/>
       <c r="H3" s="61"/>
-      <c r="I3" s="88" t="s">
+      <c r="I3" s="129" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="89"/>
-      <c r="K3" s="109" t="str">
+      <c r="J3" s="96"/>
+      <c r="K3" s="147" t="str">
         <f>IF(ISBLANK(tgpserial),"",tgpserial)</f>
         <v/>
       </c>
-      <c r="L3" s="89"/>
+      <c r="L3" s="96"/>
       <c r="M3" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="90" t="str">
+      <c r="N3" s="130" t="str">
         <f>IF(ISBLANK(dtcmission),"",dtcmission)</f>
         <v/>
       </c>
-      <c r="O3" s="91"/>
-      <c r="S3" s="149" t="s">
+      <c r="O3" s="131"/>
+      <c r="S3" s="92" t="s">
         <v>130</v>
       </c>
-      <c r="T3" s="149"/>
+      <c r="T3" s="92"/>
       <c r="V3" s="1" t="s">
         <v>10</v>
       </c>
@@ -2408,10 +2408,10 @@
       <c r="E4" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="110" t="s">
+      <c r="F4" s="148" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="111"/>
+      <c r="G4" s="149"/>
       <c r="I4" s="44" t="s">
         <v>18</v>
       </c>
@@ -2440,8 +2440,8 @@
         <v>25</v>
       </c>
       <c r="R4" s="5"/>
-      <c r="S4" s="149"/>
-      <c r="T4" s="149"/>
+      <c r="S4" s="92"/>
+      <c r="T4" s="92"/>
       <c r="V4" t="s">
         <v>27</v>
       </c>
@@ -2462,14 +2462,14 @@
       <c r="B5" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="102" t="s">
+      <c r="C5" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="103"/>
-      <c r="E5" s="96" t="s">
+      <c r="D5" s="141"/>
+      <c r="E5" s="135" t="s">
         <v>132</v>
       </c>
-      <c r="F5" s="97"/>
+      <c r="F5" s="136"/>
       <c r="G5" s="43" t="s">
         <v>33</v>
       </c>
@@ -2482,11 +2482,11 @@
       <c r="K5" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="L5" s="115" t="s">
+      <c r="L5" s="153" t="s">
         <v>134</v>
       </c>
-      <c r="M5" s="116"/>
-      <c r="N5" s="117"/>
+      <c r="M5" s="154"/>
+      <c r="N5" s="155"/>
       <c r="O5" s="43" t="s">
         <v>40</v>
       </c>
@@ -2519,7 +2519,7 @@
         <f ca="1">IF(LEN(A7)&gt;0,((ROW(A7)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B6" s="151" t="str">
+      <c r="B6" s="75" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A7)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A7)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -2535,11 +2535,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A7)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A7)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F6" s="130" t="str">
+      <c r="F6" s="105" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A7)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A7)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G6" s="87"/>
+      <c r="G6" s="100"/>
       <c r="H6" s="37"/>
       <c r="I6" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A7)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A7)-ROW($A$7)+2)/2,0))</f>
@@ -2595,16 +2595,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A7)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A7)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C7" s="133" t="str">
+      <c r="C7" s="93" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A7)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A7)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D7" s="101"/>
-      <c r="E7" s="134" t="str">
+      <c r="D7" s="94"/>
+      <c r="E7" s="95" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A7)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A7)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A7)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F7" s="89"/>
+      <c r="F7" s="96"/>
       <c r="G7" s="33" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A7)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A7)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -2622,12 +2622,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A7)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A7)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L7" s="75" t="str">
+      <c r="L7" s="118" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A7)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A7)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A7)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A7)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A7)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M7" s="76"/>
-      <c r="N7" s="77"/>
+      <c r="M7" s="119"/>
+      <c r="N7" s="120"/>
       <c r="O7" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A7)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A7)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -2651,7 +2651,7 @@
         <f ca="1">IF(LEN(A9)&gt;0,((ROW(A9)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B8" s="152" t="str">
+      <c r="B8" s="76" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A9)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A9)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -2667,11 +2667,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A9)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A9)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F8" s="129" t="str">
+      <c r="F8" s="99" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A9)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A9)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G8" s="87"/>
+      <c r="G8" s="100"/>
       <c r="H8" s="37"/>
       <c r="I8" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A9)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A9)-ROW($A$7)+2)/2,0))</f>
@@ -2727,16 +2727,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A9)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A9)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C9" s="131" t="str">
+      <c r="C9" s="97" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A9)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A9)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D9" s="101"/>
-      <c r="E9" s="132" t="str">
+      <c r="D9" s="94"/>
+      <c r="E9" s="98" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A9)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A9)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A9)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F9" s="89"/>
+      <c r="F9" s="96"/>
       <c r="G9" s="34" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A9)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A9)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -2754,12 +2754,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A9)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A9)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L9" s="78" t="str">
+      <c r="L9" s="121" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A9)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A9)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A9)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A9)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A9)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M9" s="79"/>
-      <c r="N9" s="80"/>
+      <c r="M9" s="122"/>
+      <c r="N9" s="123"/>
       <c r="O9" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A9)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A9)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -2780,7 +2780,7 @@
         <f t="shared" ref="A10" ca="1" si="0">IF(LEN(A11)&gt;0,((ROW(A11)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B10" s="151" t="str">
+      <c r="B10" s="75" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A11)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A11)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -2796,11 +2796,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A11)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A11)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F10" s="130" t="str">
+      <c r="F10" s="105" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A11)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A11)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G10" s="87"/>
+      <c r="G10" s="100"/>
       <c r="H10" s="37"/>
       <c r="I10" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A11)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A11)-ROW($A$7)+2)/2,0))</f>
@@ -2855,16 +2855,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A11)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A11)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C11" s="133" t="str">
+      <c r="C11" s="93" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A11)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A11)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D11" s="101"/>
-      <c r="E11" s="134" t="str">
+      <c r="D11" s="94"/>
+      <c r="E11" s="95" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A11)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A11)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A11)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F11" s="89"/>
+      <c r="F11" s="96"/>
       <c r="G11" s="33" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A11)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A11)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -2882,12 +2882,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A11)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A11)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L11" s="75" t="str">
+      <c r="L11" s="118" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A11)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A11)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A11)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A11)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A11)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M11" s="76"/>
-      <c r="N11" s="77"/>
+      <c r="M11" s="119"/>
+      <c r="N11" s="120"/>
       <c r="O11" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A11)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A11)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -2908,7 +2908,7 @@
         <f t="shared" ref="A12" ca="1" si="1">IF(LEN(A13)&gt;0,((ROW(A13)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B12" s="152" t="str">
+      <c r="B12" s="76" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A13)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A13)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -2924,11 +2924,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A13)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A13)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F12" s="129" t="str">
+      <c r="F12" s="99" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A13)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A13)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G12" s="87"/>
+      <c r="G12" s="100"/>
       <c r="H12" s="37"/>
       <c r="I12" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A13)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A13)-ROW($A$7)+2)/2,0))</f>
@@ -2978,16 +2978,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A13)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A13)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C13" s="131" t="str">
+      <c r="C13" s="97" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A13)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A13)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D13" s="101"/>
-      <c r="E13" s="132" t="str">
+      <c r="D13" s="94"/>
+      <c r="E13" s="98" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A13)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A13)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A13)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F13" s="89"/>
+      <c r="F13" s="96"/>
       <c r="G13" s="34" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A13)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A13)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3005,12 +3005,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A13)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A13)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L13" s="78" t="str">
+      <c r="L13" s="121" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A13)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A13)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A13)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A13)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A13)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M13" s="79"/>
-      <c r="N13" s="80"/>
+      <c r="M13" s="122"/>
+      <c r="N13" s="123"/>
       <c r="O13" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A13)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A13)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3031,7 +3031,7 @@
         <f t="shared" ref="A14" ca="1" si="2">IF(LEN(A15)&gt;0,((ROW(A15)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B14" s="151" t="str">
+      <c r="B14" s="75" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A15)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A15)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -3047,11 +3047,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A15)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A15)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F14" s="130" t="str">
+      <c r="F14" s="105" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A15)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A15)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G14" s="87"/>
+      <c r="G14" s="100"/>
       <c r="H14" s="37"/>
       <c r="I14" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A15)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A15)-ROW($A$7)+2)/2,0))</f>
@@ -3086,7 +3086,7 @@
         <v>64</v>
       </c>
       <c r="T14" s="8">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="V14" t="s">
         <v>69</v>
@@ -3104,16 +3104,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A15)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A15)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C15" s="133" t="str">
+      <c r="C15" s="93" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A15)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A15)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D15" s="101"/>
-      <c r="E15" s="134" t="str">
+      <c r="D15" s="94"/>
+      <c r="E15" s="95" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A15)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A15)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A15)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F15" s="89"/>
+      <c r="F15" s="96"/>
       <c r="G15" s="33" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A15)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A15)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3131,12 +3131,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A15)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A15)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L15" s="75" t="str">
+      <c r="L15" s="118" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A15)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A15)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A15)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A15)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A15)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M15" s="76"/>
-      <c r="N15" s="77"/>
+      <c r="M15" s="119"/>
+      <c r="N15" s="120"/>
       <c r="O15" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A15)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A15)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3161,7 +3161,7 @@
         <f t="shared" ref="A16" ca="1" si="3">IF(LEN(A17)&gt;0,((ROW(A17)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B16" s="152" t="str">
+      <c r="B16" s="76" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A17)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A17)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -3177,11 +3177,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A17)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A17)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F16" s="129" t="str">
+      <c r="F16" s="99" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A17)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A17)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G16" s="87"/>
+      <c r="G16" s="100"/>
       <c r="H16" s="37"/>
       <c r="I16" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A17)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A17)-ROW($A$7)+2)/2,0))</f>
@@ -3235,16 +3235,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A17)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A17)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C17" s="131" t="str">
+      <c r="C17" s="97" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A17)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A17)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D17" s="101"/>
-      <c r="E17" s="132" t="str">
+      <c r="D17" s="94"/>
+      <c r="E17" s="98" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A17)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A17)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A17)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F17" s="89"/>
+      <c r="F17" s="96"/>
       <c r="G17" s="34" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A17)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A17)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3262,12 +3262,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A17)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A17)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L17" s="78" t="str">
+      <c r="L17" s="121" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A17)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A17)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A17)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A17)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A17)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M17" s="79"/>
-      <c r="N17" s="80"/>
+      <c r="M17" s="122"/>
+      <c r="N17" s="123"/>
       <c r="O17" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A17)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A17)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3292,7 +3292,7 @@
         <f t="shared" ref="A18" ca="1" si="4">IF(LEN(A19)&gt;0,((ROW(A19)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B18" s="151" t="str">
+      <c r="B18" s="75" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A19)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A19)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -3308,11 +3308,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A19)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A19)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F18" s="130" t="str">
+      <c r="F18" s="105" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A19)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A19)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G18" s="87"/>
+      <c r="G18" s="100"/>
       <c r="H18" s="37"/>
       <c r="I18" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A19)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A19)-ROW($A$7)+2)/2,0))</f>
@@ -3362,16 +3362,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A19)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A19)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C19" s="133" t="str">
+      <c r="C19" s="93" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A19)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A19)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D19" s="101"/>
-      <c r="E19" s="134" t="str">
+      <c r="D19" s="94"/>
+      <c r="E19" s="95" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A19)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A19)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A19)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F19" s="89"/>
+      <c r="F19" s="96"/>
       <c r="G19" s="33" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A19)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A19)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3389,12 +3389,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A19)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A19)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L19" s="75" t="str">
+      <c r="L19" s="118" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A19)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A19)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A19)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A19)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A19)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M19" s="76"/>
-      <c r="N19" s="77"/>
+      <c r="M19" s="119"/>
+      <c r="N19" s="120"/>
       <c r="O19" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A19)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A19)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3415,7 +3415,7 @@
         <f t="shared" ref="A20" ca="1" si="5">IF(LEN(A21)&gt;0,((ROW(A21)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B20" s="152" t="str">
+      <c r="B20" s="76" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A21)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A21)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -3431,11 +3431,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A21)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A21)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F20" s="129" t="str">
+      <c r="F20" s="99" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A21)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A21)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G20" s="87"/>
+      <c r="G20" s="100"/>
       <c r="H20" s="37"/>
       <c r="I20" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A21)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A21)-ROW($A$7)+2)/2,0))</f>
@@ -3483,16 +3483,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A21)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A21)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C21" s="131" t="str">
+      <c r="C21" s="97" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A21)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A21)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D21" s="101"/>
-      <c r="E21" s="132" t="str">
+      <c r="D21" s="94"/>
+      <c r="E21" s="98" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A21)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A21)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A21)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F21" s="89"/>
+      <c r="F21" s="96"/>
       <c r="G21" s="34" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A21)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A21)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3510,12 +3510,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A21)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A21)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L21" s="78" t="str">
+      <c r="L21" s="121" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A21)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A21)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A21)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A21)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A21)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M21" s="79"/>
-      <c r="N21" s="80"/>
+      <c r="M21" s="122"/>
+      <c r="N21" s="123"/>
       <c r="O21" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A21)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A21)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3534,7 +3534,7 @@
         <f t="shared" ref="A22" ca="1" si="6">IF(LEN(A23)&gt;0,((ROW(A23)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B22" s="151" t="str">
+      <c r="B22" s="75" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A23)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A23)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -3550,11 +3550,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A23)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A23)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F22" s="130" t="str">
+      <c r="F22" s="105" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A23)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A23)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G22" s="87"/>
+      <c r="G22" s="100"/>
       <c r="H22" s="37"/>
       <c r="I22" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A23)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A23)-ROW($A$7)+2)/2,0))</f>
@@ -3602,16 +3602,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A23)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A23)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C23" s="133" t="str">
+      <c r="C23" s="93" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A23)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A23)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D23" s="101"/>
-      <c r="E23" s="134" t="str">
+      <c r="D23" s="94"/>
+      <c r="E23" s="95" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A23)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A23)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A23)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F23" s="89"/>
+      <c r="F23" s="96"/>
       <c r="G23" s="33" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A23)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A23)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3629,12 +3629,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A23)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A23)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L23" s="75" t="str">
+      <c r="L23" s="118" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A23)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A23)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A23)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A23)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A23)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M23" s="76"/>
-      <c r="N23" s="77"/>
+      <c r="M23" s="119"/>
+      <c r="N23" s="120"/>
       <c r="O23" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A23)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A23)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3653,7 +3653,7 @@
         <f t="shared" ref="A24" ca="1" si="7">IF(LEN(A25)&gt;0,((ROW(A25)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B24" s="152" t="str">
+      <c r="B24" s="76" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A25)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A25)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -3669,11 +3669,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A25)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A25)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F24" s="129" t="str">
+      <c r="F24" s="99" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A25)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A25)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G24" s="87"/>
+      <c r="G24" s="100"/>
       <c r="H24" s="37"/>
       <c r="I24" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A25)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A25)-ROW($A$7)+2)/2,0))</f>
@@ -3721,16 +3721,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A25)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A25)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C25" s="131" t="str">
+      <c r="C25" s="97" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A25)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A25)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D25" s="101"/>
-      <c r="E25" s="132" t="str">
+      <c r="D25" s="94"/>
+      <c r="E25" s="98" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A25)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A25)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A25)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F25" s="89"/>
+      <c r="F25" s="96"/>
       <c r="G25" s="34" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A25)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A25)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3748,12 +3748,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A25)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A25)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L25" s="78" t="str">
+      <c r="L25" s="121" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A25)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A25)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A25)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A25)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A25)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M25" s="79"/>
-      <c r="N25" s="80"/>
+      <c r="M25" s="122"/>
+      <c r="N25" s="123"/>
       <c r="O25" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A25)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A25)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3772,7 +3772,7 @@
         <f t="shared" ref="A26" ca="1" si="8">IF(LEN(A27)&gt;0,((ROW(A27)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B26" s="151" t="str">
+      <c r="B26" s="75" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A27)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A27)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -3788,11 +3788,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A27)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A27)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F26" s="130" t="str">
+      <c r="F26" s="105" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A27)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A27)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G26" s="87"/>
+      <c r="G26" s="100"/>
       <c r="H26" s="37"/>
       <c r="I26" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A27)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A27)-ROW($A$7)+2)/2,0))</f>
@@ -3834,16 +3834,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A27)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A27)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C27" s="133" t="str">
+      <c r="C27" s="93" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A27)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A27)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D27" s="101"/>
-      <c r="E27" s="134" t="str">
+      <c r="D27" s="94"/>
+      <c r="E27" s="95" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A27)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A27)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A27)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F27" s="89"/>
+      <c r="F27" s="96"/>
       <c r="G27" s="33" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A27)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A27)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3861,12 +3861,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A27)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A27)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L27" s="75" t="str">
+      <c r="L27" s="118" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A27)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A27)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A27)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A27)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A27)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M27" s="76"/>
-      <c r="N27" s="77"/>
+      <c r="M27" s="119"/>
+      <c r="N27" s="120"/>
       <c r="O27" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A27)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A27)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3882,7 +3882,7 @@
         <f t="shared" ref="A28" ca="1" si="9">IF(LEN(A29)&gt;0,((ROW(A29)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B28" s="152" t="str">
+      <c r="B28" s="76" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A29)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A29)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -3898,11 +3898,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A29)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A29)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F28" s="129" t="str">
+      <c r="F28" s="99" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A29)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A29)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G28" s="87"/>
+      <c r="G28" s="100"/>
       <c r="H28" s="37"/>
       <c r="I28" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A29)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A29)-ROW($A$7)+2)/2,0))</f>
@@ -3950,16 +3950,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A29)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A29)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C29" s="131" t="str">
+      <c r="C29" s="97" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A29)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A29)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D29" s="101"/>
-      <c r="E29" s="132" t="str">
+      <c r="D29" s="94"/>
+      <c r="E29" s="98" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A29)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A29)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A29)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F29" s="89"/>
+      <c r="F29" s="96"/>
       <c r="G29" s="34" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A29)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A29)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -3977,12 +3977,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A29)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A29)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L29" s="78" t="str">
+      <c r="L29" s="121" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A29)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A29)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A29)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A29)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A29)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M29" s="79"/>
-      <c r="N29" s="80"/>
+      <c r="M29" s="122"/>
+      <c r="N29" s="123"/>
       <c r="O29" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A29)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A29)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4005,7 +4005,7 @@
         <f t="shared" ref="A30" ca="1" si="10">IF(LEN(A31)&gt;0,((ROW(A31)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B30" s="151" t="str">
+      <c r="B30" s="75" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A31)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A31)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -4021,11 +4021,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A31)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A31)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F30" s="130" t="str">
+      <c r="F30" s="105" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A31)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A31)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G30" s="87"/>
+      <c r="G30" s="100"/>
       <c r="H30" s="37"/>
       <c r="I30" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A31)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A31)-ROW($A$7)+2)/2,0))</f>
@@ -4075,16 +4075,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A31)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A31)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C31" s="133" t="str">
+      <c r="C31" s="93" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A31)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A31)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D31" s="101"/>
-      <c r="E31" s="134" t="str">
+      <c r="D31" s="94"/>
+      <c r="E31" s="95" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A31)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A31)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A31)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F31" s="89"/>
+      <c r="F31" s="96"/>
       <c r="G31" s="33" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A31)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A31)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4102,12 +4102,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A31)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A31)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L31" s="75" t="str">
+      <c r="L31" s="118" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A31)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A31)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A31)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A31)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A31)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M31" s="76"/>
-      <c r="N31" s="77"/>
+      <c r="M31" s="119"/>
+      <c r="N31" s="120"/>
       <c r="O31" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A31)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A31)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4130,7 +4130,7 @@
         <f t="shared" ref="A32" ca="1" si="11">IF(LEN(A33)&gt;0,((ROW(A33)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B32" s="152" t="str">
+      <c r="B32" s="76" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A33)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A33)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -4146,11 +4146,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A33)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A33)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F32" s="129" t="str">
+      <c r="F32" s="99" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A33)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A33)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G32" s="87"/>
+      <c r="G32" s="100"/>
       <c r="H32" s="37"/>
       <c r="I32" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A33)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A33)-ROW($A$7)+2)/2,0))</f>
@@ -4202,16 +4202,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A33)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A33)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C33" s="131" t="str">
+      <c r="C33" s="97" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A33)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A33)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D33" s="101"/>
-      <c r="E33" s="132" t="str">
+      <c r="D33" s="94"/>
+      <c r="E33" s="98" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A33)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A33)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A33)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F33" s="89"/>
+      <c r="F33" s="96"/>
       <c r="G33" s="34" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A33)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A33)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4229,12 +4229,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A33)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A33)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L33" s="78" t="str">
+      <c r="L33" s="121" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A33)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A33)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A33)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A33)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A33)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M33" s="79"/>
-      <c r="N33" s="80"/>
+      <c r="M33" s="122"/>
+      <c r="N33" s="123"/>
       <c r="O33" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A33)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A33)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4257,7 +4257,7 @@
         <f t="shared" ref="A34" ca="1" si="12">IF(LEN(A35)&gt;0,((ROW(A35)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B34" s="151" t="str">
+      <c r="B34" s="75" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A35)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A35)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -4273,11 +4273,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A35)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A35)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F34" s="130" t="str">
+      <c r="F34" s="105" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A35)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A35)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G34" s="87"/>
+      <c r="G34" s="100"/>
       <c r="H34" s="37"/>
       <c r="I34" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A35)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A35)-ROW($A$7)+2)/2,0))</f>
@@ -4323,16 +4323,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A35)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A35)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C35" s="133" t="str">
+      <c r="C35" s="93" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A35)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A35)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D35" s="101"/>
-      <c r="E35" s="134" t="str">
+      <c r="D35" s="94"/>
+      <c r="E35" s="95" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A35)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A35)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A35)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F35" s="89"/>
+      <c r="F35" s="96"/>
       <c r="G35" s="33" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A35)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A35)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4350,12 +4350,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A35)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A35)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L35" s="75" t="str">
+      <c r="L35" s="118" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A35)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A35)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A35)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A35)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A35)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M35" s="76"/>
-      <c r="N35" s="77"/>
+      <c r="M35" s="119"/>
+      <c r="N35" s="120"/>
       <c r="O35" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A35)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A35)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4372,7 +4372,7 @@
         <f t="shared" ref="A36" ca="1" si="13">IF(LEN(A37)&gt;0,((ROW(A37)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B36" s="152" t="str">
+      <c r="B36" s="76" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A37)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A37)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -4388,11 +4388,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A37)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A37)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F36" s="129" t="str">
+      <c r="F36" s="99" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A37)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A37)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G36" s="87"/>
+      <c r="G36" s="100"/>
       <c r="H36" s="37"/>
       <c r="I36" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A37)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A37)-ROW($A$7)+2)/2,0))</f>
@@ -4438,16 +4438,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A37)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A37)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C37" s="131" t="str">
+      <c r="C37" s="97" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A37)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A37)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D37" s="101"/>
-      <c r="E37" s="132" t="str">
+      <c r="D37" s="94"/>
+      <c r="E37" s="98" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A37)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A37)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A37)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F37" s="89"/>
+      <c r="F37" s="96"/>
       <c r="G37" s="34" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A37)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A37)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4465,12 +4465,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A37)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A37)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L37" s="78" t="str">
+      <c r="L37" s="121" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A37)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A37)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A37)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A37)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A37)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M37" s="79"/>
-      <c r="N37" s="80"/>
+      <c r="M37" s="122"/>
+      <c r="N37" s="123"/>
       <c r="O37" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A37)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A37)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4483,22 +4483,22 @@
       <c r="U37" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="V37" s="126" t="s">
+      <c r="V37" s="115" t="s">
         <v>99</v>
       </c>
-      <c r="W37" s="127"/>
-      <c r="X37" s="127"/>
-      <c r="Y37" s="127"/>
-      <c r="Z37" s="127"/>
-      <c r="AA37" s="127"/>
-      <c r="AB37" s="128"/>
+      <c r="W37" s="116"/>
+      <c r="X37" s="116"/>
+      <c r="Y37" s="116"/>
+      <c r="Z37" s="116"/>
+      <c r="AA37" s="116"/>
+      <c r="AB37" s="117"/>
     </row>
     <row r="38" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="31" t="str">
         <f t="shared" ref="A38" ca="1" si="14">IF(LEN(A39)&gt;0,((ROW(A39)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B38" s="151" t="str">
+      <c r="B38" s="75" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A39)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A39)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -4514,11 +4514,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A39)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A39)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F38" s="130" t="str">
+      <c r="F38" s="105" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A39)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A39)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G38" s="87"/>
+      <c r="G38" s="100"/>
       <c r="H38" s="37"/>
       <c r="I38" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A39)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A39)-ROW($A$7)+2)/2,0))</f>
@@ -4554,13 +4554,13 @@
       <c r="S38" s="26"/>
       <c r="T38" s="26"/>
       <c r="U38" s="26"/>
-      <c r="V38" s="118"/>
-      <c r="W38" s="119"/>
-      <c r="X38" s="119"/>
-      <c r="Y38" s="119"/>
-      <c r="Z38" s="119"/>
-      <c r="AA38" s="119"/>
-      <c r="AB38" s="95"/>
+      <c r="V38" s="106"/>
+      <c r="W38" s="107"/>
+      <c r="X38" s="107"/>
+      <c r="Y38" s="107"/>
+      <c r="Z38" s="107"/>
+      <c r="AA38" s="107"/>
+      <c r="AB38" s="108"/>
     </row>
     <row r="39" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="str">
@@ -4571,16 +4571,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A39)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A39)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C39" s="133" t="str">
+      <c r="C39" s="93" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A39)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A39)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D39" s="101"/>
-      <c r="E39" s="134" t="str">
+      <c r="D39" s="94"/>
+      <c r="E39" s="95" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A39)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A39)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A39)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F39" s="89"/>
+      <c r="F39" s="96"/>
       <c r="G39" s="33" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A39)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A39)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4598,12 +4598,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A39)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A39)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L39" s="75" t="str">
+      <c r="L39" s="118" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A39)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A39)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A39)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A39)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A39)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M39" s="76"/>
-      <c r="N39" s="77"/>
+      <c r="M39" s="119"/>
+      <c r="N39" s="120"/>
       <c r="O39" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A39)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A39)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4614,20 +4614,20 @@
       <c r="S39" s="26"/>
       <c r="T39" s="26"/>
       <c r="U39" s="26"/>
-      <c r="V39" s="120"/>
-      <c r="W39" s="121"/>
-      <c r="X39" s="121"/>
-      <c r="Y39" s="121"/>
-      <c r="Z39" s="121"/>
-      <c r="AA39" s="121"/>
-      <c r="AB39" s="122"/>
+      <c r="V39" s="109"/>
+      <c r="W39" s="110"/>
+      <c r="X39" s="110"/>
+      <c r="Y39" s="110"/>
+      <c r="Z39" s="110"/>
+      <c r="AA39" s="110"/>
+      <c r="AB39" s="111"/>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="str">
         <f t="shared" ref="A40" ca="1" si="15">IF(LEN(A41)&gt;0,((ROW(A41)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B40" s="152" t="str">
+      <c r="B40" s="76" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A41)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A41)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -4643,11 +4643,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A41)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A41)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F40" s="129" t="str">
+      <c r="F40" s="99" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A41)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A41)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G40" s="87"/>
+      <c r="G40" s="100"/>
       <c r="H40" s="37"/>
       <c r="I40" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A41)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A41)-ROW($A$7)+2)/2,0))</f>
@@ -4683,13 +4683,13 @@
       <c r="S40" s="26"/>
       <c r="T40" s="26"/>
       <c r="U40" s="26"/>
-      <c r="V40" s="120"/>
-      <c r="W40" s="121"/>
-      <c r="X40" s="121"/>
-      <c r="Y40" s="121"/>
-      <c r="Z40" s="121"/>
-      <c r="AA40" s="121"/>
-      <c r="AB40" s="122"/>
+      <c r="V40" s="109"/>
+      <c r="W40" s="110"/>
+      <c r="X40" s="110"/>
+      <c r="Y40" s="110"/>
+      <c r="Z40" s="110"/>
+      <c r="AA40" s="110"/>
+      <c r="AB40" s="111"/>
     </row>
     <row r="41" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="19" t="str">
@@ -4700,16 +4700,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A41)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A41)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C41" s="131" t="str">
+      <c r="C41" s="97" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A41)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A41)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D41" s="101"/>
-      <c r="E41" s="132" t="str">
+      <c r="D41" s="94"/>
+      <c r="E41" s="98" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A41)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A41)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A41)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F41" s="89"/>
+      <c r="F41" s="96"/>
       <c r="G41" s="34" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A41)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A41)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4727,12 +4727,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A41)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A41)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L41" s="78" t="str">
+      <c r="L41" s="121" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A41)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A41)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A41)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A41)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A41)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M41" s="79"/>
-      <c r="N41" s="80"/>
+      <c r="M41" s="122"/>
+      <c r="N41" s="123"/>
       <c r="O41" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A41)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A41)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4743,20 +4743,20 @@
       <c r="S41" s="26"/>
       <c r="T41" s="26"/>
       <c r="U41" s="26"/>
-      <c r="V41" s="120"/>
-      <c r="W41" s="121"/>
-      <c r="X41" s="121"/>
-      <c r="Y41" s="121"/>
-      <c r="Z41" s="121"/>
-      <c r="AA41" s="121"/>
-      <c r="AB41" s="122"/>
+      <c r="V41" s="109"/>
+      <c r="W41" s="110"/>
+      <c r="X41" s="110"/>
+      <c r="Y41" s="110"/>
+      <c r="Z41" s="110"/>
+      <c r="AA41" s="110"/>
+      <c r="AB41" s="111"/>
     </row>
     <row r="42" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="str">
         <f t="shared" ref="A42" ca="1" si="16">IF(LEN(A43)&gt;0,((ROW(A43)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B42" s="151" t="str">
+      <c r="B42" s="75" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A43)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A43)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -4772,11 +4772,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A43)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A43)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F42" s="130" t="str">
+      <c r="F42" s="105" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A43)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A43)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G42" s="87"/>
+      <c r="G42" s="100"/>
       <c r="H42" s="37"/>
       <c r="I42" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A43)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A43)-ROW($A$7)+2)/2,0))</f>
@@ -4812,13 +4812,13 @@
       <c r="S42" s="26"/>
       <c r="T42" s="26"/>
       <c r="U42" s="26"/>
-      <c r="V42" s="120"/>
-      <c r="W42" s="121"/>
-      <c r="X42" s="121"/>
-      <c r="Y42" s="121"/>
-      <c r="Z42" s="121"/>
-      <c r="AA42" s="121"/>
-      <c r="AB42" s="122"/>
+      <c r="V42" s="109"/>
+      <c r="W42" s="110"/>
+      <c r="X42" s="110"/>
+      <c r="Y42" s="110"/>
+      <c r="Z42" s="110"/>
+      <c r="AA42" s="110"/>
+      <c r="AB42" s="111"/>
     </row>
     <row r="43" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="str">
@@ -4829,16 +4829,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A43)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A43)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C43" s="133" t="str">
+      <c r="C43" s="93" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A43)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A43)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D43" s="101"/>
-      <c r="E43" s="134" t="str">
+      <c r="D43" s="94"/>
+      <c r="E43" s="95" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A43)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A43)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A43)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F43" s="89"/>
+      <c r="F43" s="96"/>
       <c r="G43" s="33" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A43)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A43)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4856,12 +4856,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A43)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A43)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L43" s="75" t="str">
+      <c r="L43" s="118" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A43)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A43)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A43)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A43)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A43)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M43" s="76"/>
-      <c r="N43" s="77"/>
+      <c r="M43" s="119"/>
+      <c r="N43" s="120"/>
       <c r="O43" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A43)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A43)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4872,20 +4872,20 @@
       <c r="S43" s="26"/>
       <c r="T43" s="26"/>
       <c r="U43" s="26"/>
-      <c r="V43" s="120"/>
-      <c r="W43" s="121"/>
-      <c r="X43" s="121"/>
-      <c r="Y43" s="121"/>
-      <c r="Z43" s="121"/>
-      <c r="AA43" s="121"/>
-      <c r="AB43" s="122"/>
+      <c r="V43" s="109"/>
+      <c r="W43" s="110"/>
+      <c r="X43" s="110"/>
+      <c r="Y43" s="110"/>
+      <c r="Z43" s="110"/>
+      <c r="AA43" s="110"/>
+      <c r="AB43" s="111"/>
     </row>
     <row r="44" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="32" t="str">
         <f t="shared" ref="A44" ca="1" si="17">IF(LEN(A45)&gt;0,((ROW(A45)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B44" s="152" t="str">
+      <c r="B44" s="76" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A45)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A45)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -4901,11 +4901,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A45)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A45)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F44" s="129" t="str">
+      <c r="F44" s="99" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A45)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A45)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G44" s="87"/>
+      <c r="G44" s="100"/>
       <c r="H44" s="37"/>
       <c r="I44" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A45)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A45)-ROW($A$7)+2)/2,0))</f>
@@ -4941,13 +4941,13 @@
       <c r="S44" s="26"/>
       <c r="T44" s="26"/>
       <c r="U44" s="26"/>
-      <c r="V44" s="120"/>
-      <c r="W44" s="121"/>
-      <c r="X44" s="121"/>
-      <c r="Y44" s="121"/>
-      <c r="Z44" s="121"/>
-      <c r="AA44" s="121"/>
-      <c r="AB44" s="122"/>
+      <c r="V44" s="109"/>
+      <c r="W44" s="110"/>
+      <c r="X44" s="110"/>
+      <c r="Y44" s="110"/>
+      <c r="Z44" s="110"/>
+      <c r="AA44" s="110"/>
+      <c r="AB44" s="111"/>
     </row>
     <row r="45" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="19" t="str">
@@ -4958,16 +4958,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A45)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A45)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C45" s="131" t="str">
+      <c r="C45" s="97" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A45)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A45)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D45" s="101"/>
-      <c r="E45" s="132" t="str">
+      <c r="D45" s="94"/>
+      <c r="E45" s="98" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A45)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A45)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A45)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F45" s="89"/>
+      <c r="F45" s="96"/>
       <c r="G45" s="34" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A45)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A45)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -4985,12 +4985,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A45)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A45)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L45" s="78" t="str">
+      <c r="L45" s="121" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A45)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A45)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A45)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A45)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A45)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M45" s="79"/>
-      <c r="N45" s="80"/>
+      <c r="M45" s="122"/>
+      <c r="N45" s="123"/>
       <c r="O45" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A45)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A45)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5001,20 +5001,20 @@
       <c r="S45" s="26"/>
       <c r="T45" s="26"/>
       <c r="U45" s="26"/>
-      <c r="V45" s="120"/>
-      <c r="W45" s="121"/>
-      <c r="X45" s="121"/>
-      <c r="Y45" s="121"/>
-      <c r="Z45" s="121"/>
-      <c r="AA45" s="121"/>
-      <c r="AB45" s="122"/>
+      <c r="V45" s="109"/>
+      <c r="W45" s="110"/>
+      <c r="X45" s="110"/>
+      <c r="Y45" s="110"/>
+      <c r="Z45" s="110"/>
+      <c r="AA45" s="110"/>
+      <c r="AB45" s="111"/>
     </row>
     <row r="46" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="31" t="str">
         <f t="shared" ref="A46" ca="1" si="18">IF(LEN(A47)&gt;0,((ROW(A47)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B46" s="151" t="str">
+      <c r="B46" s="75" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A47)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A47)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -5030,11 +5030,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A47)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A47)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F46" s="130" t="str">
+      <c r="F46" s="105" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A47)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A47)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G46" s="87"/>
+      <c r="G46" s="100"/>
       <c r="H46" s="37"/>
       <c r="I46" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A47)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A47)-ROW($A$7)+2)/2,0))</f>
@@ -5070,13 +5070,13 @@
       <c r="S46" s="26"/>
       <c r="T46" s="26"/>
       <c r="U46" s="26"/>
-      <c r="V46" s="120"/>
-      <c r="W46" s="121"/>
-      <c r="X46" s="121"/>
-      <c r="Y46" s="121"/>
-      <c r="Z46" s="121"/>
-      <c r="AA46" s="121"/>
-      <c r="AB46" s="122"/>
+      <c r="V46" s="109"/>
+      <c r="W46" s="110"/>
+      <c r="X46" s="110"/>
+      <c r="Y46" s="110"/>
+      <c r="Z46" s="110"/>
+      <c r="AA46" s="110"/>
+      <c r="AB46" s="111"/>
     </row>
     <row r="47" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="14" t="str">
@@ -5087,16 +5087,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A47)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A47)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C47" s="133" t="str">
+      <c r="C47" s="93" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A47)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A47)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D47" s="101"/>
-      <c r="E47" s="134" t="str">
+      <c r="D47" s="94"/>
+      <c r="E47" s="95" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A47)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A47)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A47)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F47" s="89"/>
+      <c r="F47" s="96"/>
       <c r="G47" s="33" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A47)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A47)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5114,12 +5114,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A47)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A47)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L47" s="75" t="str">
+      <c r="L47" s="118" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A47)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A47)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A47)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A47)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A47)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M47" s="76"/>
-      <c r="N47" s="77"/>
+      <c r="M47" s="119"/>
+      <c r="N47" s="120"/>
       <c r="O47" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A47)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A47)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5130,20 +5130,20 @@
       <c r="S47" s="26"/>
       <c r="T47" s="26"/>
       <c r="U47" s="26"/>
-      <c r="V47" s="120"/>
-      <c r="W47" s="121"/>
-      <c r="X47" s="121"/>
-      <c r="Y47" s="121"/>
-      <c r="Z47" s="121"/>
-      <c r="AA47" s="121"/>
-      <c r="AB47" s="122"/>
+      <c r="V47" s="109"/>
+      <c r="W47" s="110"/>
+      <c r="X47" s="110"/>
+      <c r="Y47" s="110"/>
+      <c r="Z47" s="110"/>
+      <c r="AA47" s="110"/>
+      <c r="AB47" s="111"/>
     </row>
     <row r="48" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="32" t="str">
         <f t="shared" ref="A48" ca="1" si="19">IF(LEN(A49)&gt;0,((ROW(A49)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B48" s="152" t="str">
+      <c r="B48" s="76" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A49)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A49)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -5159,11 +5159,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A49)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A49)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F48" s="129" t="str">
+      <c r="F48" s="99" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A49)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A49)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G48" s="87"/>
+      <c r="G48" s="100"/>
       <c r="H48" s="37"/>
       <c r="I48" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A49)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A49)-ROW($A$7)+2)/2,0))</f>
@@ -5199,13 +5199,13 @@
       <c r="S48" s="26"/>
       <c r="T48" s="26"/>
       <c r="U48" s="26"/>
-      <c r="V48" s="120"/>
-      <c r="W48" s="121"/>
-      <c r="X48" s="121"/>
-      <c r="Y48" s="121"/>
-      <c r="Z48" s="121"/>
-      <c r="AA48" s="121"/>
-      <c r="AB48" s="122"/>
+      <c r="V48" s="109"/>
+      <c r="W48" s="110"/>
+      <c r="X48" s="110"/>
+      <c r="Y48" s="110"/>
+      <c r="Z48" s="110"/>
+      <c r="AA48" s="110"/>
+      <c r="AB48" s="111"/>
     </row>
     <row r="49" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="19" t="str">
@@ -5216,16 +5216,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A49)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A49)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C49" s="131" t="str">
+      <c r="C49" s="97" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A49)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A49)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D49" s="101"/>
-      <c r="E49" s="132" t="str">
+      <c r="D49" s="94"/>
+      <c r="E49" s="98" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A49)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A49)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A49)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F49" s="89"/>
+      <c r="F49" s="96"/>
       <c r="G49" s="34" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A49)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A49)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5243,12 +5243,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A49)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A49)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L49" s="78" t="str">
+      <c r="L49" s="121" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A49)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A49)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A49)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A49)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A49)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M49" s="79"/>
-      <c r="N49" s="80"/>
+      <c r="M49" s="122"/>
+      <c r="N49" s="123"/>
       <c r="O49" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A49)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A49)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5259,20 +5259,20 @@
       <c r="S49" s="26"/>
       <c r="T49" s="26"/>
       <c r="U49" s="26"/>
-      <c r="V49" s="120"/>
-      <c r="W49" s="121"/>
-      <c r="X49" s="121"/>
-      <c r="Y49" s="121"/>
-      <c r="Z49" s="121"/>
-      <c r="AA49" s="121"/>
-      <c r="AB49" s="122"/>
+      <c r="V49" s="109"/>
+      <c r="W49" s="110"/>
+      <c r="X49" s="110"/>
+      <c r="Y49" s="110"/>
+      <c r="Z49" s="110"/>
+      <c r="AA49" s="110"/>
+      <c r="AB49" s="111"/>
     </row>
     <row r="50" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="31" t="str">
         <f t="shared" ref="A50" ca="1" si="20">IF(LEN(A51)&gt;0,((ROW(A51)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B50" s="151" t="str">
+      <c r="B50" s="75" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A51)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A51)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -5288,11 +5288,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A51)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A51)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F50" s="130" t="str">
+      <c r="F50" s="105" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A51)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A51)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G50" s="87"/>
+      <c r="G50" s="100"/>
       <c r="H50" s="37"/>
       <c r="I50" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A51)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A51)-ROW($A$7)+2)/2,0))</f>
@@ -5328,13 +5328,13 @@
       <c r="S50" s="26"/>
       <c r="T50" s="26"/>
       <c r="U50" s="26"/>
-      <c r="V50" s="120"/>
-      <c r="W50" s="121"/>
-      <c r="X50" s="121"/>
-      <c r="Y50" s="121"/>
-      <c r="Z50" s="121"/>
-      <c r="AA50" s="121"/>
-      <c r="AB50" s="122"/>
+      <c r="V50" s="109"/>
+      <c r="W50" s="110"/>
+      <c r="X50" s="110"/>
+      <c r="Y50" s="110"/>
+      <c r="Z50" s="110"/>
+      <c r="AA50" s="110"/>
+      <c r="AB50" s="111"/>
     </row>
     <row r="51" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="14" t="str">
@@ -5345,16 +5345,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A51)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A51)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C51" s="133" t="str">
+      <c r="C51" s="93" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A51)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A51)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D51" s="101"/>
-      <c r="E51" s="134" t="str">
+      <c r="D51" s="94"/>
+      <c r="E51" s="95" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A51)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A51)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A51)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F51" s="89"/>
+      <c r="F51" s="96"/>
       <c r="G51" s="33" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A51)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A51)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5372,12 +5372,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A51)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A51)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L51" s="75" t="str">
+      <c r="L51" s="118" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A51)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A51)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A51)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A51)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A51)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M51" s="76"/>
-      <c r="N51" s="77"/>
+      <c r="M51" s="119"/>
+      <c r="N51" s="120"/>
       <c r="O51" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A51)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A51)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5388,20 +5388,20 @@
       <c r="S51" s="26"/>
       <c r="T51" s="26"/>
       <c r="U51" s="26"/>
-      <c r="V51" s="120"/>
-      <c r="W51" s="121"/>
-      <c r="X51" s="121"/>
-      <c r="Y51" s="121"/>
-      <c r="Z51" s="121"/>
-      <c r="AA51" s="121"/>
-      <c r="AB51" s="122"/>
+      <c r="V51" s="109"/>
+      <c r="W51" s="110"/>
+      <c r="X51" s="110"/>
+      <c r="Y51" s="110"/>
+      <c r="Z51" s="110"/>
+      <c r="AA51" s="110"/>
+      <c r="AB51" s="111"/>
     </row>
     <row r="52" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="32" t="str">
         <f t="shared" ref="A52" ca="1" si="21">IF(LEN(A53)&gt;0,((ROW(A53)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B52" s="152" t="str">
+      <c r="B52" s="76" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A53)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A53)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -5417,11 +5417,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A53)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A53)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F52" s="129" t="str">
+      <c r="F52" s="99" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A53)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A53)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G52" s="87"/>
+      <c r="G52" s="100"/>
       <c r="H52" s="37"/>
       <c r="I52" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A53)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A53)-ROW($A$7)+2)/2,0))</f>
@@ -5457,13 +5457,13 @@
       <c r="S52" s="26"/>
       <c r="T52" s="26"/>
       <c r="U52" s="26"/>
-      <c r="V52" s="120"/>
-      <c r="W52" s="121"/>
-      <c r="X52" s="121"/>
-      <c r="Y52" s="121"/>
-      <c r="Z52" s="121"/>
-      <c r="AA52" s="121"/>
-      <c r="AB52" s="122"/>
+      <c r="V52" s="109"/>
+      <c r="W52" s="110"/>
+      <c r="X52" s="110"/>
+      <c r="Y52" s="110"/>
+      <c r="Z52" s="110"/>
+      <c r="AA52" s="110"/>
+      <c r="AB52" s="111"/>
     </row>
     <row r="53" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="19" t="str">
@@ -5474,16 +5474,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A53)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A53)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C53" s="131" t="str">
+      <c r="C53" s="97" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A53)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A53)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D53" s="101"/>
-      <c r="E53" s="132" t="str">
+      <c r="D53" s="94"/>
+      <c r="E53" s="98" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A53)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A53)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A53)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F53" s="89"/>
+      <c r="F53" s="96"/>
       <c r="G53" s="34" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A53)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A53)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5501,12 +5501,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A53)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A53)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L53" s="78" t="str">
+      <c r="L53" s="121" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A53)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A53)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A53)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A53)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A53)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M53" s="79"/>
-      <c r="N53" s="80"/>
+      <c r="M53" s="122"/>
+      <c r="N53" s="123"/>
       <c r="O53" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A53)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A53)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5517,20 +5517,20 @@
       <c r="S53" s="26"/>
       <c r="T53" s="26"/>
       <c r="U53" s="26"/>
-      <c r="V53" s="123"/>
-      <c r="W53" s="124"/>
-      <c r="X53" s="124"/>
-      <c r="Y53" s="124"/>
-      <c r="Z53" s="124"/>
-      <c r="AA53" s="124"/>
-      <c r="AB53" s="125"/>
+      <c r="V53" s="112"/>
+      <c r="W53" s="113"/>
+      <c r="X53" s="113"/>
+      <c r="Y53" s="113"/>
+      <c r="Z53" s="113"/>
+      <c r="AA53" s="113"/>
+      <c r="AB53" s="114"/>
     </row>
     <row r="54" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="31" t="str">
         <f t="shared" ref="A54" ca="1" si="22">IF(LEN(A55)&gt;0,((ROW(A55)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B54" s="151" t="str">
+      <c r="B54" s="75" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A55)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A55)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -5546,11 +5546,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A55)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A55)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F54" s="130" t="str">
+      <c r="F54" s="105" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A55)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A55)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G54" s="87"/>
+      <c r="G54" s="100"/>
       <c r="H54" s="37"/>
       <c r="I54" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A55)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A55)-ROW($A$7)+2)/2,0))</f>
@@ -5596,16 +5596,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A55)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A55)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C55" s="133" t="str">
+      <c r="C55" s="93" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A55)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A55)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D55" s="101"/>
-      <c r="E55" s="134" t="str">
+      <c r="D55" s="94"/>
+      <c r="E55" s="95" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A55)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A55)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A55)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F55" s="89"/>
+      <c r="F55" s="96"/>
       <c r="G55" s="33" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A55)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A55)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5623,12 +5623,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A55)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A55)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L55" s="75" t="str">
+      <c r="L55" s="118" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A55)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A55)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A55)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A55)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A55)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M55" s="76"/>
-      <c r="N55" s="77"/>
+      <c r="M55" s="119"/>
+      <c r="N55" s="120"/>
       <c r="O55" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A55)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A55)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5645,7 +5645,7 @@
         <f t="shared" ref="A56" ca="1" si="23">IF(LEN(A57)&gt;0,((ROW(A57)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B56" s="152" t="str">
+      <c r="B56" s="76" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A57)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A57)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -5661,11 +5661,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A57)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A57)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F56" s="129" t="str">
+      <c r="F56" s="99" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A57)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A57)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G56" s="87"/>
+      <c r="G56" s="100"/>
       <c r="H56" s="37"/>
       <c r="I56" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A57)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A57)-ROW($A$7)+2)/2,0))</f>
@@ -5711,16 +5711,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A57)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A57)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C57" s="131" t="str">
+      <c r="C57" s="97" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A57)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A57)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D57" s="101"/>
-      <c r="E57" s="132" t="str">
+      <c r="D57" s="94"/>
+      <c r="E57" s="98" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A57)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A57)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A57)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F57" s="89"/>
+      <c r="F57" s="96"/>
       <c r="G57" s="34" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A57)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A57)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5738,12 +5738,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A57)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A57)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L57" s="78" t="str">
+      <c r="L57" s="121" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A57)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A57)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A57)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A57)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A57)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M57" s="79"/>
-      <c r="N57" s="80"/>
+      <c r="M57" s="122"/>
+      <c r="N57" s="123"/>
       <c r="O57" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A57)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A57)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5760,7 +5760,7 @@
         <f t="shared" ref="A58" ca="1" si="24">IF(LEN(A59)&gt;0,((ROW(A59)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B58" s="151" t="str">
+      <c r="B58" s="75" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A59)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A59)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -5776,11 +5776,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A59)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A59)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F58" s="130" t="str">
+      <c r="F58" s="105" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A59)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A59)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G58" s="87"/>
+      <c r="G58" s="100"/>
       <c r="H58" s="37"/>
       <c r="I58" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A59)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A59)-ROW($A$7)+2)/2,0))</f>
@@ -5826,16 +5826,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A59)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A59)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C59" s="133" t="str">
+      <c r="C59" s="93" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A59)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A59)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D59" s="101"/>
-      <c r="E59" s="134" t="str">
+      <c r="D59" s="94"/>
+      <c r="E59" s="95" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A59)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A59)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A59)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F59" s="89"/>
+      <c r="F59" s="96"/>
       <c r="G59" s="33" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A59)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A59)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5853,12 +5853,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A59)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A59)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L59" s="75" t="str">
+      <c r="L59" s="118" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A59)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A59)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A59)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A59)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A59)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M59" s="76"/>
-      <c r="N59" s="77"/>
+      <c r="M59" s="119"/>
+      <c r="N59" s="120"/>
       <c r="O59" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A59)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A59)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5875,7 +5875,7 @@
         <f t="shared" ref="A60" ca="1" si="25">IF(LEN(A61)&gt;0,((ROW(A61)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B60" s="152" t="str">
+      <c r="B60" s="76" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A61)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A61)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -5891,11 +5891,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A61)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A61)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F60" s="129" t="str">
+      <c r="F60" s="99" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A61)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A61)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G60" s="87"/>
+      <c r="G60" s="100"/>
       <c r="H60" s="37"/>
       <c r="I60" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A61)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A61)-ROW($A$7)+2)/2,0))</f>
@@ -5941,16 +5941,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A61)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A61)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C61" s="131" t="str">
+      <c r="C61" s="97" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A61)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A61)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D61" s="101"/>
-      <c r="E61" s="132" t="str">
+      <c r="D61" s="94"/>
+      <c r="E61" s="98" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A61)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A61)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A61)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F61" s="89"/>
+      <c r="F61" s="96"/>
       <c r="G61" s="34" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A61)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A61)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5968,12 +5968,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A61)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A61)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L61" s="78" t="str">
+      <c r="L61" s="121" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A61)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A61)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A61)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A61)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A61)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M61" s="79"/>
-      <c r="N61" s="80"/>
+      <c r="M61" s="122"/>
+      <c r="N61" s="123"/>
       <c r="O61" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A61)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A61)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -5990,7 +5990,7 @@
         <f t="shared" ref="A62" ca="1" si="26">IF(LEN(A63)&gt;0,((ROW(A63)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B62" s="151" t="str">
+      <c r="B62" s="75" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A63)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A63)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -6006,11 +6006,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A63)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A63)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F62" s="130" t="str">
+      <c r="F62" s="105" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A63)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A63)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G62" s="87"/>
+      <c r="G62" s="100"/>
       <c r="H62" s="37"/>
       <c r="I62" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A63)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A63)-ROW($A$7)+2)/2,0))</f>
@@ -6056,16 +6056,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A63)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A63)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C63" s="133" t="str">
+      <c r="C63" s="93" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A63)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A63)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D63" s="101"/>
-      <c r="E63" s="134" t="str">
+      <c r="D63" s="94"/>
+      <c r="E63" s="95" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A63)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A63)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A63)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F63" s="89"/>
+      <c r="F63" s="96"/>
       <c r="G63" s="33" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A63)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A63)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -6083,12 +6083,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A63)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A63)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L63" s="75" t="str">
+      <c r="L63" s="118" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A63)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A63)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A63)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A63)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A63)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M63" s="76"/>
-      <c r="N63" s="77"/>
+      <c r="M63" s="119"/>
+      <c r="N63" s="120"/>
       <c r="O63" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A63)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A63)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -6105,7 +6105,7 @@
         <f t="shared" ref="A64" ca="1" si="27">IF(LEN(A65)&gt;0,((ROW(A65)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B64" s="152" t="str">
+      <c r="B64" s="76" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A65)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A65)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -6121,11 +6121,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A65)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A65)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F64" s="129" t="str">
+      <c r="F64" s="99" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A65)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A65)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G64" s="87"/>
+      <c r="G64" s="100"/>
       <c r="H64" s="37"/>
       <c r="I64" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A65)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A65)-ROW($A$7)+2)/2,0))</f>
@@ -6171,16 +6171,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A65)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A65)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C65" s="131" t="str">
+      <c r="C65" s="97" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A65)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A65)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D65" s="101"/>
-      <c r="E65" s="132" t="str">
+      <c r="D65" s="94"/>
+      <c r="E65" s="98" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A65)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A65)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A65)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F65" s="89"/>
+      <c r="F65" s="96"/>
       <c r="G65" s="34" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A65)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A65)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -6198,12 +6198,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A65)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A65)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L65" s="78" t="str">
+      <c r="L65" s="121" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A65)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A65)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A65)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A65)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A65)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M65" s="79"/>
-      <c r="N65" s="80"/>
+      <c r="M65" s="122"/>
+      <c r="N65" s="123"/>
       <c r="O65" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A65)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A65)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -6220,7 +6220,7 @@
         <f t="shared" ref="A66" ca="1" si="28">IF(LEN(A67)&gt;0,((ROW(A67)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B66" s="151" t="str">
+      <c r="B66" s="75" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A67)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A67)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -6236,11 +6236,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A67)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A67)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F66" s="130" t="str">
+      <c r="F66" s="105" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A67)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A67)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G66" s="87"/>
+      <c r="G66" s="100"/>
       <c r="H66" s="37"/>
       <c r="I66" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A67)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A67)-ROW($A$7)+2)/2,0))</f>
@@ -6286,16 +6286,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A67)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A67)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C67" s="133" t="str">
+      <c r="C67" s="93" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A67)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A67)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D67" s="101"/>
-      <c r="E67" s="134" t="str">
+      <c r="D67" s="94"/>
+      <c r="E67" s="95" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A67)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A67)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A67)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F67" s="89"/>
+      <c r="F67" s="96"/>
       <c r="G67" s="33" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A67)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A67)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -6313,12 +6313,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A67)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A67)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L67" s="75" t="str">
+      <c r="L67" s="118" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A67)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A67)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A67)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A67)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A67)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M67" s="76"/>
-      <c r="N67" s="77"/>
+      <c r="M67" s="119"/>
+      <c r="N67" s="120"/>
       <c r="O67" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A67)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A67)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -6335,7 +6335,7 @@
         <f t="shared" ref="A68" ca="1" si="29">IF(LEN(A69)&gt;0,((ROW(A69)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B68" s="152" t="str">
+      <c r="B68" s="76" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A69)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A69)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -6351,11 +6351,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A69)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A69)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F68" s="129" t="str">
+      <c r="F68" s="99" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A69)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A69)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G68" s="87"/>
+      <c r="G68" s="100"/>
       <c r="H68" s="37"/>
       <c r="I68" s="17" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A69)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A69)-ROW($A$7)+2)/2,0))</f>
@@ -6401,16 +6401,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A69)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A69)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C69" s="131" t="str">
+      <c r="C69" s="97" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A69)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A69)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D69" s="101"/>
-      <c r="E69" s="132" t="str">
+      <c r="D69" s="94"/>
+      <c r="E69" s="98" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A69)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A69)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A69)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F69" s="89"/>
+      <c r="F69" s="96"/>
       <c r="G69" s="34" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A69)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A69)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -6428,12 +6428,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A69)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A69)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L69" s="78" t="str">
+      <c r="L69" s="121" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A69)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A69)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A69)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A69)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A69)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M69" s="79"/>
-      <c r="N69" s="80"/>
+      <c r="M69" s="122"/>
+      <c r="N69" s="123"/>
       <c r="O69" s="21" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A69)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A69)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -6450,7 +6450,7 @@
         <f t="shared" ref="A70" ca="1" si="30">IF(LEN(A71)&gt;0,((ROW(A71)-ROW($A$7))/2)+1,"")</f>
         <v/>
       </c>
-      <c r="B70" s="151" t="str">
+      <c r="B70" s="75" t="str">
         <f ca="1">IF(OFFSET(tot,(ROW(A71)-ROW($A$7)+2)/2,0)="","",OFFSET(tot,(ROW(A71)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
@@ -6466,11 +6466,11 @@
         <f ca="1">IF(OFFSET(wpntype,(ROW(A71)-ROW($A$7)+2)/2,0)="","",OFFSET(wpntype,(ROW(A71)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F70" s="130" t="str">
+      <c r="F70" s="105" t="str">
         <f ca="1">IF(OFFSET(tgtname,(ROW(A71)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtname,(ROW(A71)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="G70" s="87"/>
+      <c r="G70" s="100"/>
       <c r="H70" s="37"/>
       <c r="I70" s="12" t="str">
         <f ca="1">IF(OFFSET(primenav,(ROW(A71)-ROW($A$7)+2)/2,0)="","",OFFSET(primenav,(ROW(A71)-ROW($A$7)+2)/2,0))</f>
@@ -6516,16 +6516,16 @@
         <f ca="1">IF(OFFSET(tor,(ROW(A71)-ROW($A$7)+2)/2,0)="","",OFFSET(tor,(ROW(A71)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="C71" s="133" t="str">
+      <c r="C71" s="93" t="str">
         <f ca="1">IF(OFFSET(be,(ROW(A71)-ROW($A$7)+2)/2,0)="","",UPPER(BEname)&amp;" "&amp;OFFSET(be,(ROW(A71)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="D71" s="101"/>
-      <c r="E71" s="134" t="str">
+      <c r="D71" s="94"/>
+      <c r="E71" s="95" t="str">
         <f ca="1">IF(OFFSET(tgtlat,(ROW(A71)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtlat,(ROW(A71)-ROW($A$7)+2)/2,0)&amp;"  "&amp;OFFSET(tgtlon,(ROW(A71)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="F71" s="89"/>
+      <c r="F71" s="96"/>
       <c r="G71" s="33" t="str">
         <f ca="1">IF(OFFSET(tgtelev,(ROW(A71)-ROW($A$7)+2)/2,0)="","",OFFSET(tgtelev,(ROW(A71)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -6543,12 +6543,12 @@
         <f ca="1">IF(OFFSET(alt,(ROW(A71)-ROW($A$7)+2)/2,0)="","",OFFSET(alt,(ROW(A71)-ROW($A$7)+2)/2,0))</f>
         <v/>
       </c>
-      <c r="L71" s="75" t="str">
+      <c r="L71" s="118" t="str">
         <f ca="1">IF(OFFSET(ias,(ROW(A71)-ROW($A$7)+2)/2,0)="","",OFFSET(ias,(ROW(A71)-ROW($A$7)+2)/2,0)&amp;"I        "&amp;OFFSET(tas,(ROW(A71)-ROW($A$7)+2)/2,0)&amp;"T        "&amp;OFFSET(mach,(ROW(A71)-ROW($A$7)+2)/2,0)&amp;"M        "&amp;OFFSET(gs,(ROW(A71)-ROW($A$7)+2)/2,0)&amp;"GS")</f>
         <v/>
       </c>
-      <c r="M71" s="76"/>
-      <c r="N71" s="77"/>
+      <c r="M71" s="119"/>
+      <c r="N71" s="120"/>
       <c r="O71" s="16" t="str">
         <f ca="1">IF(OFFSET(delay,(ROW(A71)-ROW($A$7)+2)/2,0)="","",OFFSET(delay,(ROW(A71)-ROW($A$7)+2)/2,0))</f>
         <v/>
@@ -6561,248 +6561,395 @@
       <c r="U71" s="26"/>
     </row>
     <row r="72" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="135" t="s">
+      <c r="A72" s="101" t="s">
         <v>100</v>
       </c>
-      <c r="B72" s="136"/>
-      <c r="C72" s="136"/>
-      <c r="D72" s="136"/>
-      <c r="E72" s="136"/>
-      <c r="F72" s="136"/>
-      <c r="G72" s="136"/>
-      <c r="H72" s="136"/>
-      <c r="I72" s="136"/>
-      <c r="J72" s="136"/>
-      <c r="K72" s="136"/>
-      <c r="L72" s="136"/>
-      <c r="M72" s="136"/>
-      <c r="N72" s="136"/>
-      <c r="O72" s="137"/>
+      <c r="B72" s="102"/>
+      <c r="C72" s="102"/>
+      <c r="D72" s="102"/>
+      <c r="E72" s="102"/>
+      <c r="F72" s="102"/>
+      <c r="G72" s="102"/>
+      <c r="H72" s="102"/>
+      <c r="I72" s="102"/>
+      <c r="J72" s="102"/>
+      <c r="K72" s="102"/>
+      <c r="L72" s="102"/>
+      <c r="M72" s="102"/>
+      <c r="N72" s="102"/>
+      <c r="O72" s="103"/>
       <c r="S72" s="26"/>
       <c r="T72" s="26"/>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A73" s="138" t="s">
+      <c r="A73" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="B73" s="146"/>
-      <c r="C73" s="147"/>
-      <c r="D73" s="147"/>
-      <c r="E73" s="147"/>
-      <c r="F73" s="147"/>
-      <c r="G73" s="148"/>
-      <c r="H73" s="154"/>
-      <c r="I73" s="138" t="s">
+      <c r="B73" s="81"/>
+      <c r="C73" s="82"/>
+      <c r="D73" s="82"/>
+      <c r="E73" s="82"/>
+      <c r="F73" s="82"/>
+      <c r="G73" s="83"/>
+      <c r="H73" s="77"/>
+      <c r="I73" s="87" t="s">
         <v>105</v>
       </c>
-      <c r="J73" s="146"/>
-      <c r="K73" s="147"/>
-      <c r="L73" s="147"/>
-      <c r="M73" s="147"/>
-      <c r="N73" s="147"/>
-      <c r="O73" s="148"/>
+      <c r="J73" s="81"/>
+      <c r="K73" s="82"/>
+      <c r="L73" s="82"/>
+      <c r="M73" s="82"/>
+      <c r="N73" s="82"/>
+      <c r="O73" s="83"/>
     </row>
     <row r="74" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="139"/>
-      <c r="B74" s="140"/>
-      <c r="C74" s="153"/>
-      <c r="D74" s="153"/>
-      <c r="E74" s="153"/>
-      <c r="F74" s="153"/>
-      <c r="G74" s="141"/>
-      <c r="H74" s="155"/>
-      <c r="I74" s="139"/>
-      <c r="J74" s="140"/>
-      <c r="K74" s="153"/>
-      <c r="L74" s="153"/>
-      <c r="M74" s="153"/>
-      <c r="N74" s="153"/>
-      <c r="O74" s="141"/>
+      <c r="A74" s="88"/>
+      <c r="B74" s="84"/>
+      <c r="C74" s="85"/>
+      <c r="D74" s="85"/>
+      <c r="E74" s="85"/>
+      <c r="F74" s="85"/>
+      <c r="G74" s="86"/>
+      <c r="H74" s="78"/>
+      <c r="I74" s="88"/>
+      <c r="J74" s="84"/>
+      <c r="K74" s="85"/>
+      <c r="L74" s="85"/>
+      <c r="M74" s="85"/>
+      <c r="N74" s="85"/>
+      <c r="O74" s="86"/>
     </row>
     <row r="75" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="73"/>
-      <c r="B75" s="140"/>
-      <c r="C75" s="153"/>
-      <c r="D75" s="153"/>
-      <c r="E75" s="153"/>
-      <c r="F75" s="153"/>
-      <c r="G75" s="141"/>
+      <c r="B75" s="84"/>
+      <c r="C75" s="85"/>
+      <c r="D75" s="85"/>
+      <c r="E75" s="85"/>
+      <c r="F75" s="85"/>
+      <c r="G75" s="86"/>
       <c r="H75" s="66"/>
       <c r="I75" s="70"/>
-      <c r="J75" s="142"/>
-      <c r="K75" s="143"/>
-      <c r="L75" s="143"/>
-      <c r="M75" s="143"/>
-      <c r="N75" s="143"/>
-      <c r="O75" s="144"/>
+      <c r="J75" s="89"/>
+      <c r="K75" s="90"/>
+      <c r="L75" s="90"/>
+      <c r="M75" s="90"/>
+      <c r="N75" s="90"/>
+      <c r="O75" s="91"/>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A76" s="145" t="s">
+      <c r="A76" s="104" t="s">
         <v>102</v>
       </c>
-      <c r="B76" s="146"/>
-      <c r="C76" s="147"/>
-      <c r="D76" s="147"/>
-      <c r="E76" s="147"/>
-      <c r="F76" s="147"/>
-      <c r="G76" s="148"/>
+      <c r="B76" s="81"/>
+      <c r="C76" s="82"/>
+      <c r="D76" s="82"/>
+      <c r="E76" s="82"/>
+      <c r="F76" s="82"/>
+      <c r="G76" s="83"/>
       <c r="H76" s="37"/>
-      <c r="I76" s="138" t="s">
+      <c r="I76" s="87" t="s">
         <v>106</v>
       </c>
-      <c r="J76" s="146"/>
-      <c r="K76" s="147"/>
-      <c r="L76" s="147"/>
-      <c r="M76" s="147"/>
-      <c r="N76" s="147"/>
-      <c r="O76" s="148"/>
+      <c r="J76" s="81"/>
+      <c r="K76" s="82"/>
+      <c r="L76" s="82"/>
+      <c r="M76" s="82"/>
+      <c r="N76" s="82"/>
+      <c r="O76" s="83"/>
     </row>
     <row r="77" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="139"/>
-      <c r="B77" s="140"/>
-      <c r="C77" s="153"/>
-      <c r="D77" s="153"/>
-      <c r="E77" s="153"/>
-      <c r="F77" s="153"/>
-      <c r="G77" s="141"/>
-      <c r="H77" s="155"/>
-      <c r="I77" s="139"/>
-      <c r="J77" s="140"/>
-      <c r="K77" s="153"/>
-      <c r="L77" s="153"/>
-      <c r="M77" s="153"/>
-      <c r="N77" s="153"/>
-      <c r="O77" s="141"/>
+      <c r="A77" s="88"/>
+      <c r="B77" s="84"/>
+      <c r="C77" s="85"/>
+      <c r="D77" s="85"/>
+      <c r="E77" s="85"/>
+      <c r="F77" s="85"/>
+      <c r="G77" s="86"/>
+      <c r="H77" s="78"/>
+      <c r="I77" s="88"/>
+      <c r="J77" s="84"/>
+      <c r="K77" s="85"/>
+      <c r="L77" s="85"/>
+      <c r="M77" s="85"/>
+      <c r="N77" s="85"/>
+      <c r="O77" s="86"/>
     </row>
     <row r="78" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="73"/>
-      <c r="B78" s="140"/>
-      <c r="C78" s="153"/>
-      <c r="D78" s="153"/>
-      <c r="E78" s="153"/>
-      <c r="F78" s="153"/>
-      <c r="G78" s="141"/>
+      <c r="B78" s="84"/>
+      <c r="C78" s="85"/>
+      <c r="D78" s="85"/>
+      <c r="E78" s="85"/>
+      <c r="F78" s="85"/>
+      <c r="G78" s="86"/>
       <c r="H78" s="37"/>
       <c r="I78" s="70"/>
-      <c r="J78" s="142"/>
-      <c r="K78" s="143"/>
-      <c r="L78" s="143"/>
-      <c r="M78" s="143"/>
-      <c r="N78" s="143"/>
-      <c r="O78" s="144"/>
+      <c r="J78" s="89"/>
+      <c r="K78" s="90"/>
+      <c r="L78" s="90"/>
+      <c r="M78" s="90"/>
+      <c r="N78" s="90"/>
+      <c r="O78" s="91"/>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A79" s="81" t="s">
+      <c r="A79" s="79" t="s">
         <v>103</v>
       </c>
-      <c r="B79" s="146"/>
-      <c r="C79" s="147"/>
-      <c r="D79" s="147"/>
-      <c r="E79" s="147"/>
-      <c r="F79" s="147"/>
-      <c r="G79" s="148"/>
+      <c r="B79" s="81"/>
+      <c r="C79" s="82"/>
+      <c r="D79" s="82"/>
+      <c r="E79" s="82"/>
+      <c r="F79" s="82"/>
+      <c r="G79" s="83"/>
       <c r="H79" s="37"/>
-      <c r="I79" s="138" t="s">
+      <c r="I79" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="J79" s="146"/>
-      <c r="K79" s="147"/>
-      <c r="L79" s="147"/>
-      <c r="M79" s="147"/>
-      <c r="N79" s="147"/>
-      <c r="O79" s="148"/>
+      <c r="J79" s="81"/>
+      <c r="K79" s="82"/>
+      <c r="L79" s="82"/>
+      <c r="M79" s="82"/>
+      <c r="N79" s="82"/>
+      <c r="O79" s="83"/>
     </row>
     <row r="80" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="150"/>
-      <c r="B80" s="140"/>
-      <c r="C80" s="153"/>
-      <c r="D80" s="153"/>
-      <c r="E80" s="153"/>
-      <c r="F80" s="153"/>
-      <c r="G80" s="141"/>
-      <c r="H80" s="155"/>
-      <c r="I80" s="139"/>
-      <c r="J80" s="140"/>
-      <c r="K80" s="153"/>
-      <c r="L80" s="153"/>
-      <c r="M80" s="153"/>
-      <c r="N80" s="153"/>
-      <c r="O80" s="141"/>
+      <c r="A80" s="80"/>
+      <c r="B80" s="84"/>
+      <c r="C80" s="85"/>
+      <c r="D80" s="85"/>
+      <c r="E80" s="85"/>
+      <c r="F80" s="85"/>
+      <c r="G80" s="86"/>
+      <c r="H80" s="78"/>
+      <c r="I80" s="88"/>
+      <c r="J80" s="84"/>
+      <c r="K80" s="85"/>
+      <c r="L80" s="85"/>
+      <c r="M80" s="85"/>
+      <c r="N80" s="85"/>
+      <c r="O80" s="86"/>
     </row>
     <row r="81" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="72"/>
-      <c r="B81" s="140"/>
-      <c r="C81" s="153"/>
-      <c r="D81" s="153"/>
-      <c r="E81" s="153"/>
-      <c r="F81" s="153"/>
-      <c r="G81" s="141"/>
+      <c r="B81" s="84"/>
+      <c r="C81" s="85"/>
+      <c r="D81" s="85"/>
+      <c r="E81" s="85"/>
+      <c r="F81" s="85"/>
+      <c r="G81" s="86"/>
       <c r="H81" s="37"/>
       <c r="I81" s="70"/>
-      <c r="J81" s="142"/>
-      <c r="K81" s="143"/>
-      <c r="L81" s="143"/>
-      <c r="M81" s="143"/>
-      <c r="N81" s="143"/>
-      <c r="O81" s="144"/>
+      <c r="J81" s="89"/>
+      <c r="K81" s="90"/>
+      <c r="L81" s="90"/>
+      <c r="M81" s="90"/>
+      <c r="N81" s="90"/>
+      <c r="O81" s="91"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A82" s="81" t="s">
+      <c r="A82" s="79" t="s">
         <v>104</v>
       </c>
-      <c r="B82" s="146"/>
-      <c r="C82" s="147"/>
-      <c r="D82" s="147"/>
-      <c r="E82" s="147"/>
-      <c r="F82" s="147"/>
-      <c r="G82" s="148"/>
+      <c r="B82" s="81"/>
+      <c r="C82" s="82"/>
+      <c r="D82" s="82"/>
+      <c r="E82" s="82"/>
+      <c r="F82" s="82"/>
+      <c r="G82" s="83"/>
       <c r="H82" s="37"/>
-      <c r="I82" s="138" t="s">
+      <c r="I82" s="87" t="s">
         <v>108</v>
       </c>
-      <c r="J82" s="146"/>
-      <c r="K82" s="147"/>
-      <c r="L82" s="147"/>
-      <c r="M82" s="147"/>
-      <c r="N82" s="147"/>
-      <c r="O82" s="148"/>
+      <c r="J82" s="81"/>
+      <c r="K82" s="82"/>
+      <c r="L82" s="82"/>
+      <c r="M82" s="82"/>
+      <c r="N82" s="82"/>
+      <c r="O82" s="83"/>
     </row>
     <row r="83" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="150"/>
-      <c r="B83" s="140"/>
-      <c r="C83" s="153"/>
-      <c r="D83" s="153"/>
-      <c r="E83" s="153"/>
-      <c r="F83" s="153"/>
-      <c r="G83" s="141"/>
-      <c r="H83" s="155"/>
-      <c r="I83" s="139"/>
-      <c r="J83" s="140"/>
-      <c r="K83" s="153"/>
-      <c r="L83" s="153"/>
-      <c r="M83" s="153"/>
-      <c r="N83" s="153"/>
-      <c r="O83" s="141"/>
+      <c r="A83" s="80"/>
+      <c r="B83" s="84"/>
+      <c r="C83" s="85"/>
+      <c r="D83" s="85"/>
+      <c r="E83" s="85"/>
+      <c r="F83" s="85"/>
+      <c r="G83" s="86"/>
+      <c r="H83" s="78"/>
+      <c r="I83" s="88"/>
+      <c r="J83" s="84"/>
+      <c r="K83" s="85"/>
+      <c r="L83" s="85"/>
+      <c r="M83" s="85"/>
+      <c r="N83" s="85"/>
+      <c r="O83" s="86"/>
     </row>
     <row r="84" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="74"/>
-      <c r="B84" s="142"/>
-      <c r="C84" s="143"/>
-      <c r="D84" s="143"/>
-      <c r="E84" s="143"/>
-      <c r="F84" s="143"/>
-      <c r="G84" s="144"/>
+      <c r="B84" s="89"/>
+      <c r="C84" s="90"/>
+      <c r="D84" s="90"/>
+      <c r="E84" s="90"/>
+      <c r="F84" s="90"/>
+      <c r="G84" s="91"/>
       <c r="H84" s="67"/>
       <c r="I84" s="71"/>
-      <c r="J84" s="142"/>
-      <c r="K84" s="143"/>
-      <c r="L84" s="143"/>
-      <c r="M84" s="143"/>
-      <c r="N84" s="143"/>
-      <c r="O84" s="144"/>
+      <c r="J84" s="89"/>
+      <c r="K84" s="90"/>
+      <c r="L84" s="90"/>
+      <c r="M84" s="90"/>
+      <c r="N84" s="90"/>
+      <c r="O84" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="171">
+    <mergeCell ref="L45:N45"/>
+    <mergeCell ref="L47:N47"/>
+    <mergeCell ref="L49:N49"/>
+    <mergeCell ref="L51:N51"/>
+    <mergeCell ref="L53:N53"/>
+    <mergeCell ref="L55:N55"/>
+    <mergeCell ref="L57:N57"/>
+    <mergeCell ref="L59:N59"/>
+    <mergeCell ref="L61:N61"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="L29:N29"/>
+    <mergeCell ref="L31:N31"/>
+    <mergeCell ref="L33:N33"/>
+    <mergeCell ref="L35:N35"/>
+    <mergeCell ref="L37:N37"/>
+    <mergeCell ref="L39:N39"/>
+    <mergeCell ref="L41:N41"/>
+    <mergeCell ref="L43:N43"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="V38:AB53"/>
+    <mergeCell ref="V37:AB37"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="L21:N21"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="L25:N25"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="B73:G75"/>
+    <mergeCell ref="I73:I74"/>
+    <mergeCell ref="J73:O75"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="B76:G78"/>
+    <mergeCell ref="I76:I77"/>
+    <mergeCell ref="J76:O78"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="L63:N63"/>
+    <mergeCell ref="L65:N65"/>
+    <mergeCell ref="L67:N67"/>
+    <mergeCell ref="L69:N69"/>
+    <mergeCell ref="L71:N71"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="A72:O72"/>
     <mergeCell ref="A79:A80"/>
     <mergeCell ref="B79:G81"/>
     <mergeCell ref="I79:I80"/>
@@ -6827,173 +6974,26 @@
     <mergeCell ref="C55:D55"/>
     <mergeCell ref="E55:F55"/>
     <mergeCell ref="C57:D57"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="A72:O72"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="B73:G75"/>
-    <mergeCell ref="I73:I74"/>
-    <mergeCell ref="J73:O75"/>
-    <mergeCell ref="A76:A77"/>
-    <mergeCell ref="B76:G78"/>
-    <mergeCell ref="I76:I77"/>
-    <mergeCell ref="J76:O78"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="V38:AB53"/>
-    <mergeCell ref="V37:AB37"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="L19:N19"/>
-    <mergeCell ref="L21:N21"/>
-    <mergeCell ref="L23:N23"/>
-    <mergeCell ref="L25:N25"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="L29:N29"/>
-    <mergeCell ref="L31:N31"/>
-    <mergeCell ref="L33:N33"/>
-    <mergeCell ref="L35:N35"/>
-    <mergeCell ref="L37:N37"/>
-    <mergeCell ref="L39:N39"/>
-    <mergeCell ref="L41:N41"/>
-    <mergeCell ref="L43:N43"/>
-    <mergeCell ref="L63:N63"/>
-    <mergeCell ref="L65:N65"/>
-    <mergeCell ref="L67:N67"/>
-    <mergeCell ref="L69:N69"/>
-    <mergeCell ref="L71:N71"/>
-    <mergeCell ref="L45:N45"/>
-    <mergeCell ref="L47:N47"/>
-    <mergeCell ref="L49:N49"/>
-    <mergeCell ref="L51:N51"/>
-    <mergeCell ref="L53:N53"/>
-    <mergeCell ref="L55:N55"/>
-    <mergeCell ref="L57:N57"/>
-    <mergeCell ref="L59:N59"/>
-    <mergeCell ref="L61:N61"/>
   </mergeCells>
   <conditionalFormatting sqref="O6 O10 O14 O18 O22 O26 O30 O34 O38 O42 O46 O50 O54 O58 O62 O66 O70">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="13" priority="4">
       <formula>O6="Unachiev"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="12" priority="5">
       <formula>OR(O6="ZONE",O6="LAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="11" priority="6">
       <formula>O6="RANGE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O8 O12 O16 O20 O24 O28 O32 O36 O40 O44 O48 O52 O56 O60 O64 O68">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>O8="Unachiev"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>OR(O8="ZONE",O8="LAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula>O8="RANGE"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>